<commit_message>
Created more Data for Usecases
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/UseCaseCourseData.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/UseCaseCourseData.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1FC3C-A22A-4415-83FC-557038DC4941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FD449C-DAFA-4602-AAA2-F6B64AC054B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="2724" windowWidth="40428" windowHeight="22476" xr2:uid="{42E46E1E-8980-4662-AB6D-571AD8C791C7}"/>
+    <workbookView xWindow="2940" yWindow="345" windowWidth="23115" windowHeight="19830" activeTab="1" xr2:uid="{42E46E1E-8980-4662-AB6D-571AD8C791C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="2" r:id="rId1"/>
     <sheet name="Course" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Course!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Course!$A$1:$W$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="309">
   <si>
     <t>CourseProviderId</t>
   </si>
@@ -407,13 +407,776 @@
   </si>
   <si>
     <t>APOLLO Weiterbildungen</t>
+  </si>
+  <si>
+    <t>Biwe</t>
+  </si>
+  <si>
+    <t>USECASE</t>
+  </si>
+  <si>
+    <t>PartialQualification</t>
+  </si>
+  <si>
+    <t>InPerson</t>
+  </si>
+  <si>
+    <t>FullTime</t>
+  </si>
+  <si>
+    <t>https://www.biwe-bbq.de/weiterbildungen/anzeige/tq-lagerlogistik</t>
+  </si>
+  <si>
+    <t>DE-DE</t>
+  </si>
+  <si>
+    <t>KeyPhrases</t>
+  </si>
+  <si>
+    <t>Bei der Teilqualifizierung wird der anerkannte Ausbildungsberuf Fachkraft für Lagerlogistik (m/w/d) in folgende Module aufgegliedert.
+TQ-Modul 1 - Wareneingang (11 Wochen, davon 3 Wochen im Unternehmen)
+Annehmen der Güter, Entladen und Kontrollieren der Lieferung, Prüfen der Lieferung anhand der Begleitpapiere, Abschluss Flurförderschein
+TQ-Modul 2 - Lagerung (11 Wochen, davon 3 Wochen im Unternehmen)
+Auspacken, Sortieren und Lagern der Güter anforderungsgerecht und nach wirtschaftlichen Grundsätzen unter Beachtung der Lagerordnung , Transportieren und Zuleiten der Güter zum betrieblichen Bestimmungsort
+TQ-Modul 3 - Innerbetriebliche Logistik und Kontrolle (11 Wochen, davon 3 Wochen im Unternehmen)
+Anwenden betrieblicher Informations- und Kommunikationssysteme, Standardsoftware und arbeitsplatzbezogener Software, Anwenden fachspezifischer Fremdsprachenkenntnisse, Durchführen von Bestandskontrollen und Maßnahmen der Bestandspflege
+TQ-Modul 4 - Kommissionierung und Endkontrolle (11 Wochen, davon 3 Wochen im Unternehmen)
+Erstellen von Ladelisten/Beladeplänen unter Beachtung von Ladevorschriften, Kennzeichnen, Beschriften und Sichern von Sendungen nach gesetzlichen Vorgaben, Kommissionieren und Verpacken der Güter für Sendungen und Zusammenstellen zu Ladeeinheiten
+TQ-Modul 5 - Versand (11 Wochen, davon 3 Wochen im Unternehmen)
+Kennzeichnen, Beschriften und Sichern von Sendungen nach gesetzlichen Vorgaben, Bearbeiten der Versand- und Begleitpapiere und Erstellen von Versandaufzeichnungen
+TQ-Modul 6 - Arbeitsorganisation und Qualitätssicherung (11 Wochen, davon 3 Wochen im Unternehmen)
+Mitwirken bei logistischen Planungs- und Organisationsprozessen, Mitwirken bei qualitätssichernden Maßnahmen, Planen, Organisieren und Überwachen des Einsatzes von Arbeits- und Fördermitteln</t>
+  </si>
+  <si>
+    <t>Arbeitssuchende und Beschäftigte, die keinen oder einen fachfremden Berufsabschluss haben und sich weiter qualifizieren möchten und einen anerkannten Berufsabschluss anstreben.</t>
+  </si>
+  <si>
+    <t>Mindestens Sprachniveau B1 (wünschenswert B2), hohe Lernmotivation und Konzentrationsfähigkeit, Kommunikationsfähigkeit, Führerschein. Die Eignung wird in einem persönlichen Beratungsgespräch geprüft</t>
+  </si>
+  <si>
+    <t>Die TQ unterstützt Sie beim Einstieg in den Beruf Fachkraft für Lagerlogistik (m/w/d) und gibt Ihnen die Chance auf einen höher qualifizierten Arbeitsplatz. Überschaubare Lernphasen durch fachspezifische Ausrichtung der einzelnen Module, ermöglichen ein flexibles Lernen.</t>
+  </si>
+  <si>
+    <t>Bei erfolgreicher Kompetenzfeststellung erhalten Sie nach jedem Modul ein Zertifikat inklusive Kompetenzfeststellungsergebnis, das bundesweit anerkannt ist.</t>
+  </si>
+  <si>
+    <t>Förderfähig durch einen Bildungsgutschein, die Deutsche Rentenversicherung Bund und Land sowie das Qualifizierungschancengesetz</t>
+  </si>
+  <si>
+    <t>&lt;Label TextType=\"Html\"&gt;\r\n    &lt;![CDATA[\r\n       &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ec66b111-d8d0-4516-88ba-ee0b6fe6f695\" target=\"_blank\"&gt;Kundenbestellungen bearbeiten&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/27536739-c38b-45d2-9e96-1573b1d32fdd\" target=\"_blank\"&gt;Verpackungszubehör nutzen&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/5d2e82cc-5943-4218-a459-a1956fad2b63\" target=\"_blank\"&gt;Lagerbestand verwalten&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d5fa1ed6-6cd8-41b9-8e78-2ba168ff3457\" target=\"_blank\"&gt;Bestellungen aus dem Online-Geschäft bearbeiten&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/7838de1e-d65e-4a3f-b60b-e2213026116f\" target=\"_blank\"&gt;Geräte für den Materialtransport bedienen&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ab2bb44a-3956-4028-8715-8b70b1960b99\" target=\"_blank\"&gt;schwere Gewichte heben&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/e0ae0101-ab8f-47a2-938b-ab0cc367b3b5\" target=\"_blank\"&gt;Lagerdatenbank pflegen&lt;/a&gt;.\r\n   \t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/5b91b6d4-345e-4195-a078-218514871e7b\" target=\"_blank\"&gt;effiziente Nutzung von Lagerraum sicherstellen&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/28b7d7fb-0483-4877-9aaa-f990f10f16f5\" target=\"_blank\"&gt;Pick-by-Voice-Kommissionierungssysteme bedienen&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/b2b8ec41-d6d1-470d-9e78-4eee515aaa3d\" target=\"_blank\"&gt;Kettensäge bedienen&lt;/a&gt;.\r\n\t   &lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/23db1cab-e565-4a90-89f8-3a8685a20029\" target=\"_blank\"&gt;den physischen Zustand des Lagers pflegen und aufrechterhalten&lt;/a&gt;.   \r\n    ]]&gt;\r\n &lt;/Label&gt;</t>
+  </si>
+  <si>
+    <t>Bbw</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90527/fachlageristin</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – Tqdigital</t>
+  </si>
+  <si>
+    <t>Mit der Teilqualifizierung können Sie Schritt für Schritt in sechs Etappen den Berufsabschluss Fachkraft für Lagerlogistik (m/w/d) erreichen. Bei erfolgreicher Kompetenzfeststellung erhalten Sie nach jeder Etappe ein Zertifikat inklusive Kompetenzfeststellungsergebnis, das bundesweit anerkannt ist. Sie haben die Möglichkeit, sich zur Externenprüfung bei der zuständigen Kammer anzumelden und damit den Berufsabschluss zu erwerben.</t>
+  </si>
+  <si>
+    <t>Arbeitsorganisation im Betreib
+Einsatz von Arbeitsmitteln (Wiegen und Messen)
+Wareneingang - Annahme von Gütern
+Lagerung von Gütern
+Kommissionierung und Verpackung
+Versand von Gütern
+Sicherheits- und Gesundheitsschutz, Umweltschutz
+Logistische Prozesse und Qualitätssicherung
+Die vermittelten Unterrichtsinhalte werden in der Praxis vertieft und in ausbildungsberechtigten Betrieben in der Region erweitert.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>Arbeitssuchende
+Menschen ohne Berufsabschluss
+Beschäftigte
+Migrant*innen/Asylbewerber*innen
+Menschen mit Behinderung
+Soldat*innen</t>
+  </si>
+  <si>
+    <t>Hauptschulabschluss, technisches Grundverständnis
+Berufsabschluss oder mindestens dreijährige berufliche
+Praxis
+gute Deutschkenntnisse in Wort und Schrift
+Beratungsgespräch und bei Bedarf ein Eignungstest</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Teilnahme an der Umschulung sind Sie Fachlagerist*in.</t>
+  </si>
+  <si>
+    <t>IHK-Abschluss
+Prüfung vor der zuständigen Kammer
+Träger-Zertifikat</t>
+  </si>
+  <si>
+    <t>Bfz</t>
+  </si>
+  <si>
+    <t>Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss Fachlagerist*in
+Als Fachlagerist*in sind Sie unter anderem in Bereichen wie der Warenannahme oder dem Lager tätig. Im Modul 1 Güterbewegung und Arbeitsschutz lernen Sie Grundlagen über den Arbeitsschutz, Umweltschutz und rechtliche Grundlagen kennen. Mit dieser Teilqualifizierung machen Sie den ersten Schritt, hin zu einem anerkannten Berufsabschluss, zu dem Sie sich mit weiteren Modulen qualifizieren können.</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Teilnahme an diesem Modul beherrschen Sie die Güterbewegung und den Arbeitsschutz der Teilqualifizierung "Fachlagerist*in".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teilqualifizierungen bieten Ihnen die Möglichkeit, in einzelnen Abschnitten Fachkenntnisse zu erwerben und sich diese Leistungen zertifizieren zu lassen. Wenn alle Module eines Berufs erfolgreich absolviert werden, ist eine Externenprüfung vor der zuständigen Kammer möglich.
+Mit der Teilqualifizierung können Sie sich Schritt für Schritt in fünf Modulen zum*zur Fachlagerist*in mit IHK-Kammerprüfung qualifizieren. </t>
+  </si>
+  <si>
+    <t>Einführung in das Berufsfeld und Vermittlung von Grundlagenwissen
+Arbeitsschutz
+Umweltschutz und rechtliche Grundlagen
+Güter im Betrieb transportieren
+Flurförderschein
+Das Gütesiegel „Eine TQ besser!" der ARBEITGEBERINITIATIVE TEILQUALIFIZIERUNG garantiert die Durchführung von Teilqualifizierungen nach festgelegten Standards.
+Nach erfolgreicher Kompetenzfeststellung erhalten Sie das bfz vbw Zertifikat Teilqualifizierung Fachlagerist*in, Modul 1: Güterbewegung und Arbeitsschutz.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>Agentur für Arbeit
+Berufsförderungsdienst der Bundeswehr
+Berufsgenossenschaften
+Bildungsgutschein (BGS)
+Jobcenter
+Knappschaft-Bahn-See
+Qualifizierungschancengesetz
+Renten- und Unfallversicherungsträger
+Selbstzahler - individuelle Fördermöglichkeiten
+Transfergesellschaften</t>
+  </si>
+  <si>
+    <t>Folgende Voraussetzungen müssen Sie für die Teilqualifizierung mitbringen:
+- ausreichendes Sprachniveau (mind. B1, B2 in der digitalen Lernform),
+- hohe Lernmotivation,
+- sowohl technisches wie auch kaufmännisches Grundverständnis
+- Interesse an einer Arbeitsaufnahme im Lagerbereich
+Ihre Eignung prüfen wir gemeinsam mit Ihnen in einem persönlichen Beratungsgespräch.</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90580/fachlageristin-wareneingang-modul-2</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90531/fachlageristin-gueterbewegung-und-arbeitsschutz-modul-1</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – WARENEINGANG (MODUL 2)</t>
+  </si>
+  <si>
+    <t>Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss Fachlagerist*in
+Als Fachlagerist*in nehmen Sie unter anderem Waren an und lagern diese dann sachgerecht. Außerdem machen Sie Lieferungen versandfertig oder leiten Güter an Empfänger im Betrieb weiter. Im Modul 2 Wareneingang wird Ihnen Wissen über die Güterannahme und Güterkontrolle, sowie das Tabellenkalkulations- und Lagerhaltungsprogramm vermittelt. Mit dieser Teilqualifizierung stellen Sie die Weichen hin zu einem anerkannten Berufsabschluss, für den Sie sich mit weiteren Modulen qualifizieren können.</t>
+  </si>
+  <si>
+    <t>Die betriebliche Qualifizierungsphase von 4 Wochen erfolgt bei Betrieben in der Region. 
+Inhalte
+Grundlagen Beschaffung
+Güter annehmen und kontrollieren
+Tabellenkalkulations- und Lagerhaltungsprogramm
+Erfolgsunterstützung, Kompetenzfeststellung praktisch und theoretisch
+Das Gütesiegel „Eine TQ besser!" der ARBEITGEBERINITIATIVE TEILQUALIFIZIERUNG garantiert die Durchführung von Teilqualifizierungen nach festgelegten Standards.
+Nach erfolgreicher Kompetenzfeststellung erhalten Sie das bfz vbw Zertifikat Teilqualifizierung Fachlagerist*in, Modul 2: Wareneingang.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90041/fachlageristin-lagerhaltung-und-warenpflege-modul-3</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90871/fachlageristin-gueterverladung-und-versand-modul-5</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90405/fachlageristin-kommissionierung-und-verpackung-modul-4</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – KOMMISSIONIERUNG UND VERPACKUNG (MODUL 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss Fachlagerist*in
+Als Fachlagerist*in sind Sie unter anderem für die Annahme von Waren an und die sachgerechte Lagerung zuständig. Des Weiteren stellen Sie Lieferungen für den bereit oder leiten Güter an Empfänger im Betrieb weiter. Dieses Modul vermittelt Ihnen Kenntnisse über die Kommissionierung und die Verpackung. Mit dieser Teilqualifizierung bestreiten Sie einen wichtigen Teil des Weges zu einem anerkannten Berufsabschluss, zu dem Sie sich mit weiteren Modulen qualifizieren können.
+</t>
+  </si>
+  <si>
+    <t>Die betriebliche Qualifizierungsphase von 4 Wochen erfolgt bei Betrieben in der Region. 
+Inhalte
+Güter kommissionieren
+Güter verpacken
+Das Gütesiegel „Eine TQ besser!" der ARBEITGEBERINITIATIVE TEILQUALIFIZIERUNG garantiert die Durchführung von Teilqualifizierungen nach festgelegten Standards.
+Nach erfolgreicher Kompetenzfeststellung erhalten Sie das bfz vbw Zertifikat Teilqualifizierung Fachlagerist*in, Modul 4: Kommissionierung und Verpackung.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Teilnahme an diesem Modul beherrschen Sie die Kommissionierung und Verpackung der Teilqualifizierung "Fachlagerist*in"</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Teilnahme an diesem Modul beherrschen Sie die Lagerhaltung und Warenpflege der Teilqualifizierung "Fachlagerist*in".</t>
+  </si>
+  <si>
+    <t>Nach erfolgreicher Teilnahme an diesem Modul beherrschen Sie die Güterverladung und Versand der Teilqualifizierung "Fachlagerist*in"</t>
+  </si>
+  <si>
+    <t>Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss Fachlagerist*in
+Als Fachlagerist*in sind Sie für die Warenannahmen und deren sachgerechte Lagerung verantwortlich. Zudem stellen Sie zum Beispiel Lieferungen zum weiteren Versand zusammen oder leiten Güter an Empfänger im Betrieb weiter. In diesem Modul lernen Sie die Grundlagen über die Optimierung von logistischen Prozesse und die Güterbearbeitung kennen. Mit dieser Teilqualifizierung gehen Sie einen wichtigen Schritt hin zu einem anerkannten Berufsabschluss, zu dem Sie sich mit weiteren Modulen qualifizieren können.</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – LAGERHALTUNG UND WARENPFLEGE (MODUL 3)</t>
+  </si>
+  <si>
+    <t>Mit der Teilqualifizierung können Sie sich Schritt für Schritt in fünf Modulen zum*zur Fachlagerist*in mit IHK-Kammerprüfung qualifizieren. 
+Die betriebliche Qualifizierungsphase von 4 Wochen erfolgt bei Betrieben in der Region. 
+Inhalte
+Güter lagern
+Güter bearbeiten inkl. Inventur
+Logistische Prozesse optimieren (Grundlagen)
+Kennzahlen ermitteln und auswerten (Grundlagen)
+Das Gütesiegel „Eine TQ besser!" der ARBEITGEBERINITIATIVE TEILQUALIFIZIERUNG garantiert die Durchführung von Teilqualifizierungen nach festgelegten Standards.
+Nach erfolgreicher Kompetenzfeststellung erhalten Sie das bfz vbw Zertifikat Teilqualifizierung Fachlagerist*in, Modul 3: Lagerhaltung und Warenpflege.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – GÜTERVERLADUNG UND VERSAND (MODUL 5)</t>
+  </si>
+  <si>
+    <t>Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss Fachlagerist*in
+Als Fachlagerist*in nehmen Sie unter anderem Waren an und lagern diese sachgerecht. Sie machen des Weiteren Lieferungen versandfertig oder leiten verschiedene Güter an Empfänger im Betrieb weiter. Güter verladen und versenden sind die Hauptinhalte von diesem Modul 5. Mit dieser Teilqualifizierung stellen Sie die Weichen für einen anerkannten Berufsabschluss, für dem Sie sich mit weiteren Modulen qualifizieren können.</t>
+  </si>
+  <si>
+    <t>Teilqualifizierungen bieten Ihnen die Möglichkeit, in einzelnen Abschnitten Fachkenntnisse zu erwerben und sich diese Leistungen zertifizieren zu lassen. Wenn alle Module eines Berufsbildes erfolgreich absolviert werden, ist eine Externenprüfung vor der zuständigen Kammer möglich. 
+Mit der Teilqualifizierung können Sie sich Schritt für Schritt in fünf Modulen zum*zur Fachlagerist*in mit IHK-Kammerprüfung qualifizieren.
+Die betriebliche Qualifizierungsphase von 4 Wochen erfolgt bei Betrieben in der Region. 
+Inhalte
+Güter verladen inkl. Ladungssicherung
+Güter versenden
+Das Gütesiegel „Eine TQ besser!" der ARBEITGEBERINITIATIVE TEILQUALIFIZIERUNG garantiert die Durchführung von Teilqualifizierungen nach festgelegten Standards.
+Nach erfolgreicher Kompetenzfeststellung erhalten Sie das bfz vbw Zertifikat Teilqualifizierung Fachlagerist*in, Modul 5: Güterverladung und Versand.
+Hinweis zu unseren Lernmethoden
+Live-​Online-Unterricht
+Der Unterricht findet ausschließlich online statt – mit einem*r Dozent*in im virtuellen Klassenzimmer (Adobe Connect, Vitero o. Ä.).
+Unsere Lernprozessbegleiter*innen unterstützen Sie im kompletten Schulungszeitraum.
+Sie wollen die Qualifizierung von zu Hause aus machen? Hierzu benötigen Sie die Zustimmung des Kostenträgers. Bei digitalen Umschulungen ist zusätzlich das Einverständnis der regionalen Kammer erforderlich.</t>
+  </si>
+  <si>
+    <t>Tuev</t>
+  </si>
+  <si>
+    <t>Im Lager werden Produkte gelagert und umgeschlagen, kommissioniert, konfektioniert, verpackt, zum Versand vorbereitet oder auch Retouren bearbeitet. Mit diesem Seminar erhalten Sie einen fundierten und praxisorientierten Einblick in die Aufgaben der Lager- und Materialwirtschaft bei der betrieblichen Leistungserstellung und die wichtigsten Abwicklungsprozesse in der Lagerlogistik. Damit verfügen Sie über das notwendige "Handwerkszeug" für Ihre täglichen, operativen Aufgaben in einer modernen betrieblichen Lagerlogistik.</t>
+  </si>
+  <si>
+    <t>Grundlagen der Lagerwirtschaft kompakt.</t>
+  </si>
+  <si>
+    <t>https://akademie.tuv.com/weiterbildungen/grundlagen-der-lagerwirtschaft-kompakt-557431</t>
+  </si>
+  <si>
+    <t>Lagermitarbeiter mit ersten praktischen Berufserfahrungen, Nachwuchskräfte sowie Quereinsteiger im Bereich Lager, Materialwirtschaft und Logistik.</t>
+  </si>
+  <si>
+    <t>Sie erhalten das notwendige Grundlagenwissen zum Einstieg in die komplexe Welt der Lagerlogistik.
+Sie lernen alle im Lager zu verrichtenden Tätigkeiten und Prozesse vom Wareneingang über die Lagerung, Kommissionierung bis zum Versand anhand vieler praktischer Beispiele kennen.
+Mit der Teilnahme legen Sie das Fundament für Ihre erfolgreiche Tätigkeit in der betrieblichen Lagerlogistik und für einen weiteren Ausbau Ihrer Handlungskompetenz im operativen Alltag.</t>
+  </si>
+  <si>
+    <t>1. Die Lagerwirtschaft im Unternehmen
+- Bedeutung und Aufgaben
+- Lagerprozesse im Überblick
+2. Lagersysteme und Lagertechnik
+- Flurfördermittel
+- Lagermittel
+- Verpackungseinheiten
+- Lagerverwaltung und -steuerung
+- Wearables: Pick-by-Vision, Pick-by-Voice
+- Automatisierung im Lager - Ausblick Industrie 4.0
+3. Unfallverhütung
+- Gefahrenquellen im Lager
+- Potentiell Gefahren beim Transport erkennen
+- Gefahren vermeiden
+- Fehler erkennen und vermeiden
+- Richtiges Verhalten bei Unfällen
+4. Lagern im Logistikprozess
+- Lagerfunktionen
+- Lagertypen
+- Lagerhalter
+5. Prozesse im Lager
+- Wareneingang
+- Wareneingangskontrolle
+- Ware einlagern
+- Ware lagern
+6. Auftragsabwicklung und Kommissionierung
+- Auftrag annehmen und kommissionieren
+- Auftrag zusammenstellen und versandfertig machen
+7. Warenausgang
+- Ware verpacken und sichern
+- Ware verladen und versenden
+8. Warenbestände
+- Ware identifizieren und buchen
+- Inventur durchführen
+- Bestandsarten
+9. Die Wichtigkeit von Ordnung und Sauberkeit10. Wirtschaftlichkeitsfaktor Lager
+- Ausgleichsfunktionen und Aufgaben
+- Anforderungen und Kosten
+11. Prozesse verbessern
+- Kennzahlen in der Lagerlogistik
+- Vermeidung von Fehlern im Lager
+- Was kann ich dazu beitragen?</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>ab 1.300,00 €
+Nettopreis (zzgl. MwSt.)
+ab 1.547,00 €
+Bruttopreis (inkl. MwSt.)</t>
+  </si>
+  <si>
+    <t>ContactId</t>
+  </si>
+  <si>
+    <t>ContactMail</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>ContactPhone</t>
+  </si>
+  <si>
+    <t>info-stuttgart@biwe.de</t>
+  </si>
+  <si>
+    <t>BBQ Stuttgart</t>
+  </si>
+  <si>
+    <t>0711 252875-19</t>
+  </si>
+  <si>
+    <t>OnAndOffline</t>
+  </si>
+  <si>
+    <t>https://www.bbw-seminare.de/seminarinfos/eca/10647/fachkraft-fuer-lagerlogistik-ihk/</t>
+  </si>
+  <si>
+    <t>Berufsbegleitende Nachqualifizierung mit Vorbereitung auf die Externenprüfung (IHK)
+Im Lehrgang „Fachkraft für Lagerlogistik mit Vorbereitung auf die Externenprüfung (IHK)“ werden die Teilnehmer auf das Tätigkeitsprofil des Fachlageristen vorbereitet. Das Lehrgangskonzept beinhaltet zudem alle relevanten Inhalte für die Teilnahme an der Externenprüfung zum Erwerb des Berufsabschlusses „Fachkraft für Lagerlogistik (IHK)“.</t>
+  </si>
+  <si>
+    <t>Inhalte
+Wirtschafts- und Sozialkunde 
+Sicherheit und Gesundheitsschutz bei der Arbeit, Umweltschutz 
+Arbeitsorganisation, Information und Kommunikation
+Güterkontrolle und qualitätssichernde Maßnahmen 
+Buchführung 
+Annahme von Gütern 
+Lagerung von Gütern 
+Kommissionierung und Verpackung von Gütern 
+Versand von Gütern
+Lagerung/Warenpflege 
+Prozesse der Lagerlogistik 
+Rationeller und qualitätssichernder Güterumschlag 
+Intensive Prüfungsvorbereitung auf die 3 Teile der Theorieprüfung
+Intensive Prüfungsvorbereitung auf die praktische und die schriftlich-praktische Prüfung</t>
+  </si>
+  <si>
+    <t>Der Lehrgang richtet sich speziell an Mitarbeiter, die keinen oder einen fachfremden Berufsabschluss haben, aber einschlägige betriebliche Praxiserfahrung im Lager- oder Logistikbereich mitbringen. Auf diesem Praxiswissen aufbauend werden die Inhalte der Ausbildung in einem kompakten Lehrgang berufsbegleitend vermittelt.</t>
+  </si>
+  <si>
+    <t>Arbeitsagentur
+BA-Förderung nach dem Qualifizierungschancengesetz für Beschäftigte</t>
+  </si>
+  <si>
+    <t>Voraussetzungen
+Geringqualifizierte (Ungelernte ohne Berufsabschluss oder Berufs-entfremdete die mehr als 4 Jahre nicht im erlernten Beruf tätig sind)
+Zum Zeitpunkt der Anmeldung zur IHK-Prüfung muss eine viereinhalb-jährige Tätigkeit im Lager- bzw. Logistikbereich nachgewiesen werden</t>
+  </si>
+  <si>
+    <t>Mira Bernhart</t>
+  </si>
+  <si>
+    <t>mira.bernhart@bbw.de</t>
+  </si>
+  <si>
+    <t>+499317973261</t>
+  </si>
+  <si>
+    <t>Termin1 Start</t>
+  </si>
+  <si>
+    <t>Termin1 Ende</t>
+  </si>
+  <si>
+    <t>Termin2 Start</t>
+  </si>
+  <si>
+    <t>Termin2 Ende</t>
+  </si>
+  <si>
+    <t>Termin3 Start</t>
+  </si>
+  <si>
+    <t>Termin3 Ende</t>
+  </si>
+  <si>
+    <t>14.06.2023</t>
+  </si>
+  <si>
+    <t>16.06.2023</t>
+  </si>
+  <si>
+    <t>+4980013535577</t>
+  </si>
+  <si>
+    <t>servicecenter@de.tuv.com</t>
+  </si>
+  <si>
+    <t>Service Center</t>
+  </si>
+  <si>
+    <t>Christine Ziegler</t>
+  </si>
+  <si>
+    <t>07391 58751-13</t>
+  </si>
+  <si>
+    <t>christine.ziegler@bfz.de</t>
+  </si>
+  <si>
+    <t>13.02.2023</t>
+  </si>
+  <si>
+    <t>19.05.2023</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90531/fachlageristin-gueterbewegung-und-arbeitsschutz-modul-1?r%5Bl%5D%5Bd%5D=50&amp;r%5Bl%5D%5Bl%5D=71634%20Ludwigsburg</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90580/fachlageristin-wareneingang-modul-2?r%5Bl%5D%5Bd%5D=50&amp;r%5Bl%5D%5Bl%5D=71634%20Ludwigsburg#box_eventlist</t>
+  </si>
+  <si>
+    <t>Link Termin</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90041/fachlageristin-lagerhaltung-und-warenpflege-modul-3?r%5Bl%5D%5Bd%5D=50&amp;r%5Bl%5D%5Bl%5D=71634%20Ludwigsburg%20#box_eventlist</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90405/fachlageristin-kommissionierung-und-verpackung-modul-4?r%5Bl%5D%5Bd%5D=50&amp;r%5Bl%5D%5Bl%5D=71634%20Ludwigsburg#box_eventlist</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90871/fachlageristin-gueterverladung-und-versand-modul-5?r%5Bl%5D%5Bd%5D=50&amp;r%5Bl%5D%5Bl%5D=71634%20Ludwigsburg%20#box_eventlist</t>
+  </si>
+  <si>
+    <t>07.06.2024</t>
+  </si>
+  <si>
+    <t>13 Wochen , Vollzeit</t>
+  </si>
+  <si>
+    <t>16 Monate, Vollzeit</t>
+  </si>
+  <si>
+    <t>25.08.2023</t>
+  </si>
+  <si>
+    <t>12 Wochen , Vollzeit</t>
+  </si>
+  <si>
+    <t>Fachkraft für Lagerlogistik (IHK)</t>
+  </si>
+  <si>
+    <t>06.02.2023</t>
+  </si>
+  <si>
+    <t>12.05.2023</t>
+  </si>
+  <si>
+    <t>Hinweis Preis: Bei Förderung durch die Agentur für Arbeit mit einem Bildungsgutschein ist der Lehrgang kostenfrei!</t>
+  </si>
+  <si>
+    <t>22.05.2023</t>
+  </si>
+  <si>
+    <t>23.01.2023</t>
+  </si>
+  <si>
+    <t>28.04.2023</t>
+  </si>
+  <si>
+    <t>15.05.2023</t>
+  </si>
+  <si>
+    <t>04.08.2023</t>
+  </si>
+  <si>
+    <t>02.05.2023</t>
+  </si>
+  <si>
+    <t>21.07.2023</t>
+  </si>
+  <si>
+    <t>21.08.2023</t>
+  </si>
+  <si>
+    <t>24.11.2023</t>
+  </si>
+  <si>
+    <t>https://akademie.tuv.com/weiterbildungen/praxiswissen-wareneingang-aufbau-workshop-fuer-lagerleiter-473630</t>
+  </si>
+  <si>
+    <t>Praxiswissen Wareneingang - Aufbau-Workshop für Lagerleiter.</t>
+  </si>
+  <si>
+    <t>Verbesserungspotenziale erkennen, Servicequalität optimieren und Logistikkosten reduzieren.
+Abwicklungsfehler und organisatorische Mängel im Wareneingang nehmen direkten Einfluss auf alle folgenden logistischen Prozesse und können wesentliche Ursache für hohe Logistikkosten und schlechte Servicequalität sein. Unser Workshop hilft Ihnen, komplexe Verantwortlichkeiten im Abwicklungsprozess Ihres Wareneingangs richtig einzuordnen und diese mit modernen Methoden umzusetzen.</t>
+  </si>
+  <si>
+    <t>UnPublishingDate</t>
+  </si>
+  <si>
+    <t>01.12.2022</t>
+  </si>
+  <si>
+    <t>Fachkraft für Lagerlogistik - TQ</t>
+  </si>
+  <si>
+    <t>FACHLAGERIST*IN – GÜTERBEWEGUNG UND ARBEITSSCHUTZ (MODUL 1)</t>
+  </si>
+  <si>
+    <t>Lagerleiter, Fach- und Führungskräfte aus Wareneingang, Lager, Versand, Materialwirtschaft und Logistik.</t>
+  </si>
+  <si>
+    <t>Sie kennen die grundlegenden Aufgaben des Wareneingangs und wissen diese gezielt mit den notwendigen Instrumenten und Methoden im operativen Tagesgeschäft umzusetzen.
+Sie erhalten einen umfassenden, praxisbezogenen Leitfaden, um Teilprozesse im Wareneingang zu optimieren und Abweichungen zu korrigieren.
+Sie erreichen logistische Zielgrößen wie niedrige Bestände, kurze Durchlaufzeiten, Termintreue und guten Lieferservice mit geeigneten Methoden und wissen diese nachhaltig sicherzustellen.
+Sie berücksichtigen die Akteure im betrieblichen Leistungsprozess und verbessern damit nachhaltig die Material-, Informations- und Kommunikationsschnittstellen.</t>
+  </si>
+  <si>
+    <t>ab 975,00 €
+Nettopreis (zzgl. MwSt.)
+ab 1.160,25 €
+Bruttopreis (inkl. MwSt.)</t>
+  </si>
+  <si>
+    <t>5 Module je 11 Wochen</t>
+  </si>
+  <si>
+    <t>68 Wochen</t>
+  </si>
+  <si>
+    <t>11 Wochen</t>
+  </si>
+  <si>
+    <t>13 Wochen</t>
+  </si>
+  <si>
+    <t>12 Wochen</t>
+  </si>
+  <si>
+    <t>3 Tage</t>
+  </si>
+  <si>
+    <t>2 Tage</t>
+  </si>
+  <si>
+    <t>06.11.2023</t>
+  </si>
+  <si>
+    <t>08.11.2023</t>
+  </si>
+  <si>
+    <t>07.02.2023</t>
+  </si>
+  <si>
+    <t>30.11.2023</t>
+  </si>
+  <si>
+    <t>01.12.2023</t>
+  </si>
+  <si>
+    <t>Fachlagerist m/w/d Teilqualifizierung</t>
+  </si>
+  <si>
+    <t>Fachlageristen nehmen Waren an und lagern diese sachgerecht. Sie stellen Lieferungen für den Versand zusammen bzw. leiten Güter an die entsprechenden Stellen im Betrieb weiter. Der IHK-Berufsabschluss Fachlagerist wird in 5 Teilqualifizierungen (TQ) zerlegt. Dies ermöglicht die Kombination aus Beschäftigungs- und Qualifizierungsphasen.
+TQ5: Versand
+-	Fachtheorie: Güter verladen und Güter versenden
+-	Fachpraxis: Ladegewicht und benötigten Frachtraum ermitteln
+-	Fachpraxis: Verladung der zusammengestellten Ware unter Beachtung der Ladevorschriften</t>
+  </si>
+  <si>
+    <t>Sofort / Individueller Einstieg</t>
+  </si>
+  <si>
+    <t>Dauer nach Vorgabe (3 bis 6 Monate)</t>
+  </si>
+  <si>
+    <t>Präsenz</t>
+  </si>
+  <si>
+    <t>Förderbar über Bildungsgutschein</t>
+  </si>
+  <si>
+    <t>KAUFMANN*FRAU IM E-​COMMERCE – WARENWIRTSCHAFT UND ONLINEVERTRIEB (MODUL 1)</t>
+  </si>
+  <si>
+    <t>Teilqualifizierung zur schrittweisen Qualifizierung bis zum Berufsabschluss E-Commerce
+Als Kaufmann*frau im E-Commerce verkaufen Sie Produkte und Dienstleistungen über das Internet. Im Modul Warenwirtschaft und Onlinevertrieb lernen Sie unter anderem Online-Vertriebskanäle auszuwählen und einzusetzen. Mit dieser Teilqualifizierung legen Sie den ersten Schritt zurück, hin zu einem anerkannten Berufsabschluss, zu dem Sie sich mit weiteren Modulen qualifizieren können.</t>
+  </si>
+  <si>
+    <t>Beschäftigte
+Arbeitssuchende
+Berufsrückkehrer*innen
+Menschen ohne Berufsabschluss</t>
+  </si>
+  <si>
+    <t>Folgende Voraussetzungen müssen Sie für die Teilqualifizierung mitbringen:
+- Sprachniveau B2
+- hohe Lernmotivation und Konzentrationsfähigkeit,
+- Grundkenntnisse bzw. Grundverständnis im kaufmännischen Bereich.
+Ihre Eignung prüfen wir gemeinsam mit Ihnen in einem persönlichen Beratungsgespräch.</t>
+  </si>
+  <si>
+    <t>07.07.2023</t>
+  </si>
+  <si>
+    <t>Ismail Debre</t>
+  </si>
+  <si>
+    <t>ismail.debre@bfz.de</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90512/kaufmannfrau-im-e-commerce-5-module</t>
+  </si>
+  <si>
+    <t>Mindestens Sprachniveau B1 (wünschenswert B2), hohe Lernmotivation und Konzentrationsfähigkeit, Grundkenntnisse bzw. Grundverständnis im kaufmännischen Bereich. Die Eignung wird in einem persönlichen Beratungsgespräch geprüft</t>
+  </si>
+  <si>
+    <t>Die TQ unterstützt Sie beim Einstieg in den Beruf Kaufmann im E-Commerce (m/w/d) und gibt Ihnen die Chance auf einen höher qualifizierten Arbeitsplatz. Überschaubare Lernphasen durch fachspezifische Ausrichtung der einzelnen Module, ermöglichen ein flexibles Lernen.</t>
+  </si>
+  <si>
+    <t>5 Module je 15 Wochen</t>
+  </si>
+  <si>
+    <t>https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-ecommerce-hybrid</t>
+  </si>
+  <si>
+    <t>15 Wochen</t>
+  </si>
+  <si>
+    <t>Kaufmann im E-Commerce - TQ</t>
+  </si>
+  <si>
+    <t>Kaufmann im E-Commerce - TQ (Modul 1)</t>
+  </si>
+  <si>
+    <t>Sie lernen bequem von zuhause aus oder bei uns vor Ort (Hybrid-Kurs)
+Mit der Teilqualifizierung können Sie Schritt für Schritt in sechs Etappen den Berufsabschluss Kaufmann im E-Commerce (m/w/d) erreichen. Bei erfolgreicher Kompetenzfeststellung erhalten Sie nach jeder Etappe ein Zertifikat inklusive Kompetenzfeststellungsergebnis, das bundesweit anerkannt ist. Sie haben die Möglichkeit, sich zur Externenprüfung bei der zuständigen Kammer anzumelden und damit den Berufsabschluss zu erwerben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://esco.ec.europa.eu/de/classification/occupation?uri=http%3A//data.europa.eu/esco/occupation/cd94def5-3442-4c2e-ae3d-0761a3008bcb </t>
+  </si>
+  <si>
+    <t>info-bbq@biwe.de</t>
+  </si>
+  <si>
+    <t>BBQ Bildung und Berufliche Qualifizierung gGmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+49 (0)711 135340-0  </t>
+  </si>
+  <si>
+    <t>Kaufmann*frau im E-​Commerce (5 Module)</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs/eca-90154/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1?r%5Bl%5D%5Bd%5D=25&amp;r%5Bl%5D%5Bl%5D=81929%20M%C3%BCnchen#box_eventlist</t>
+  </si>
+  <si>
+    <t>beratung@bfz.de</t>
+  </si>
+  <si>
+    <t>24 Monate, Vollzeit</t>
+  </si>
+  <si>
+    <t>19 Wochen</t>
+  </si>
+  <si>
+    <t>Teilzeit, Vollzeit möglich https://www.bfz.de/kurs/eca-90154/pdf/90154-23-001-4/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1.pdf https://www.bfz.de/kurs/eca-90154/pdf/90154-23-003-4/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teilqualifizierung zur schrittweisen Vorbereitung auf den Berufsabschluss E-Commerce
+Als Kaufmann*frau im E-Commerce verkaufen Sie Produkte und Dienstleistungen über das Internet. Mit dieser Teilqualifizierung legen Sie den ersten Schritt zurück, hin zu einem anerkannten Berufsabschluss, zu dem Sie sich mit Hilfe dieser Module qualifizieren können. </t>
+  </si>
+  <si>
+    <t>Umschulung im digitalen Lernformat in Vollzeit
+Als Fachlagerist*in nehmen Sie Waren an und lagern sie sachgerecht. Zudem stellen Sie Lieferungen für den Versand zusammen oder leiten Güter an Empfänger im Betrieb weiter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modularmaßnahme E – Commerce - Modul 1 Online Vertrieb </t>
+  </si>
+  <si>
+    <t>4 Monate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie haben eine kaufmännische Ausbildung und wollen Ihr Qualifikationsprofil um den Bereich des E-Commerce erweitern? Dann ist diese Weiterbildung das Richtige für Sie.　 
+Der Onlinehandel ist eine Zukunftsbranche, die stetig weiterwächst. Immer mehr Unternehmen bauen ihr Online-Angebot aus und suchen dafür nach qualifizierten Fachkräften. Mitarbeiter: innen im E-Commerce betreuen Verkaufs- und Kaufprozesse von Waren oder Dienstleistungen im Internet und Online-Kundenservice. Sie haben Aufgaben im Einkauf, Werbung, Logistik oder auch in der IT. Auch die Kommunikation mit Kunden rund um Beratung, Bestellung und Reklamationen, die Auswahl und Pflege von Webshops oder virtuellen Marktplätzen können zu ihren Aufgaben gehören. </t>
+  </si>
+  <si>
+    <t>Förderung über Bildungsgutschein möglich, Förderung über Qualifizierungschancengesetz (für Arbeitnehmer) -&gt; Kosten werden über Förderung übernommen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.01.2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.05.2023 </t>
+  </si>
+  <si>
+    <t>0221 806-9000</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://www.bbw-seminare.de/inhouse-angebote/</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kontakt</t>
+  </si>
+  <si>
+    <t>https://akademie.tuv.com/ueber-die-akademie</t>
+  </si>
+  <si>
+    <t>https://www.biwe-bbq.de/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,8 +1222,81 @@
       <name val="MesloLGM NF"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF666666"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +1306,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,7 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -544,6 +1404,57 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -861,18 +1772,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAAAA66-7B9A-4A00-A3EB-59B446683C3F}">
   <dimension ref="A1:BO14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="BD1" sqref="BD1"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BE2" sqref="BE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -1075,7 +1986,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1151,7 +2062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1196,7 +2107,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:67" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1241,7 +2152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:67" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1286,7 +2197,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:67" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1331,7 +2242,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:67">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1372,7 +2283,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:67">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1413,7 +2324,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:67">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1454,7 +2365,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:67">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1495,7 +2406,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:67">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1536,7 +2447,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:67">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1577,7 +2488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:67">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1618,7 +2529,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:67">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1671,117 +2582,1603 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D671E26-080C-462D-901A-35D8ED7721D2}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="109.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="18"/>
+    <col min="26" max="26" width="14" style="18" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.28515625" style="21" customWidth="1"/>
+    <col min="32" max="32" width="16.42578125" customWidth="1"/>
+    <col min="33" max="36" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:37" s="13" customFormat="1" ht="18.75">
+      <c r="A1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" s="13" t="s">
         <v>18</v>
       </c>
+      <c r="W1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG1" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="16.5" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" t="s">
+        <v>134</v>
+      </c>
+      <c r="U2" t="s">
+        <v>135</v>
+      </c>
+      <c r="V2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" ht="15" customHeight="1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA3">
+        <v>101</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" ht="15" customHeight="1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M4" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" t="s">
+        <v>247</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA4">
+        <v>101</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="15" customHeight="1">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" t="s">
+        <v>156</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA5">
+        <v>101</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD5" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="15" customHeight="1">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M6" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" t="s">
+        <v>169</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y6" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z6" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA6">
+        <v>101</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD6" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE6" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="15" customHeight="1">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N7" t="s">
+        <v>162</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z7" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA7">
+        <v>101</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD7" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE7" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="15" customHeight="1">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="M8" t="s">
+        <v>128</v>
+      </c>
+      <c r="N8" t="s">
+        <v>171</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z8" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA8">
+        <v>101</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD8" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE8" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>239</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="15" customHeight="1">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M9" t="s">
+        <v>128</v>
+      </c>
+      <c r="N9" t="s">
+        <v>228</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="V9" s="22"/>
+      <c r="Y9" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA9">
+        <v>102</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD9" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK9" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="15" customHeight="1">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="D10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M10" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" t="s">
+        <v>176</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="R10" s="12"/>
+      <c r="T10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="V10" s="23"/>
+      <c r="X10" s="16">
+        <v>1547</v>
+      </c>
+      <c r="Y10" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z10" s="19"/>
+      <c r="AA10">
+        <v>201</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD10" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>258</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>259</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" s="25" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="25">
+        <v>1</v>
+      </c>
+      <c r="B11" s="25">
+        <v>201</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="T11" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="X11" s="29">
+        <v>1160.25</v>
+      </c>
+      <c r="Y11" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA11" s="25">
+        <v>201</v>
+      </c>
+      <c r="AB11" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC11" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD11" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE11" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF11" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="AG11" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AH11" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="15" customHeight="1">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>202</v>
+      </c>
+      <c r="D12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" t="s">
+        <v>267</v>
+      </c>
+      <c r="I12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N12" t="s">
+        <v>263</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="R12" s="10"/>
+      <c r="U12" t="s">
+        <v>268</v>
+      </c>
+      <c r="X12" s="31">
+        <v>2245</v>
+      </c>
+      <c r="AE12" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="AK12" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" s="33" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="33">
+        <v>2</v>
+      </c>
+      <c r="B13" s="33">
+        <v>30</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="K13" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="M13" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="N13" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="O13" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q13" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="R13" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="S13" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="T13" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="U13" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="V13" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA13" s="33">
+        <v>30</v>
+      </c>
+      <c r="AB13" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC13" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD13" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE13" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK13" s="40" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="38">
+        <v>2</v>
+      </c>
+      <c r="B14" s="38">
+        <v>31</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="K14" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="L14" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q14" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="R14" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="S14" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="T14" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U14" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="V14" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA14" s="38">
+        <v>30</v>
+      </c>
+      <c r="AB14" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC14" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD14" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE14" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK14" s="40" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="15" customHeight="1">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="M15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N15" t="s">
+        <v>289</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V15" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA15">
+        <v>130</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AK15" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="15" customHeight="1">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M16" t="s">
+        <v>128</v>
+      </c>
+      <c r="N16" t="s">
+        <v>269</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V16" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y16" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA16">
+        <v>130</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE16" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" ht="15" customHeight="1">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>230</v>
+      </c>
+      <c r="D17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="M17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" t="s">
+        <v>297</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="U17" t="s">
+        <v>300</v>
+      </c>
+      <c r="X17" s="31"/>
+      <c r="AD17" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE17" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>302</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="X18" s="31"/>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="X19" s="31"/>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="X20" s="31"/>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="X21" s="31"/>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="X22" s="31"/>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="X23" s="31"/>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="X24" s="31"/>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="X25" s="31"/>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="X26" s="31"/>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="X27" s="31"/>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="X28" s="31"/>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="X29" s="31"/>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="X30" s="31"/>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="X31" s="31"/>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="X32" s="31"/>
+    </row>
+    <row r="33" spans="24:24">
+      <c r="X33" s="31"/>
+    </row>
+    <row r="34" spans="24:24">
+      <c r="X34" s="31"/>
+    </row>
+    <row r="35" spans="24:24">
+      <c r="X35" s="31"/>
+    </row>
+    <row r="36" spans="24:24">
+      <c r="X36" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S1" xr:uid="{4D671E26-080C-462D-901A-35D8ED7721D2}"/>
+  <autoFilter ref="A1:W1" xr:uid="{4D671E26-080C-462D-901A-35D8ED7721D2}"/>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{8CC932C3-7FF1-4CBE-AC5F-95D1BAEB23AF}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{ACC795F6-27FB-4197-8E77-BAE6FD4B0977}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{CBF31EA4-BAC3-4796-BE40-CEC49FABEC17}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{1D9E1721-DB68-45F1-90B7-29871AB19B58}"/>
+    <hyperlink ref="L4" r:id="rId5" xr:uid="{70E61FC4-8007-404D-AEF8-FA2202FCAE72}"/>
+    <hyperlink ref="L5" r:id="rId6" xr:uid="{6326C6C4-846F-445B-94B9-39AA99BD3A59}"/>
+    <hyperlink ref="L6" r:id="rId7" xr:uid="{AAFAB3C4-B342-4536-997A-0499A8339412}"/>
+    <hyperlink ref="L8" r:id="rId8" xr:uid="{A87129C6-742E-4634-8EF7-9D02FE56ECE4}"/>
+    <hyperlink ref="L7" r:id="rId9" xr:uid="{DC2E6AD3-0F1C-4C39-8E22-ECF39C842305}"/>
+    <hyperlink ref="L10" r:id="rId10" xr:uid="{962798D7-DDB3-4B72-8B32-A21A9CC92FDD}"/>
+    <hyperlink ref="K10" r:id="rId11" xr:uid="{6A91C522-B523-4DCF-8EBC-EB217DAFD8EE}"/>
+    <hyperlink ref="K9" r:id="rId12" xr:uid="{EC2B592D-886B-4EB9-98C9-E47522CA1664}"/>
+    <hyperlink ref="L9" r:id="rId13" xr:uid="{08438625-AA4C-4A90-95C3-FFD691995563}"/>
+    <hyperlink ref="AB9" r:id="rId14" xr:uid="{32840A4E-0CD2-4B19-A0A2-603207BD0F39}"/>
+    <hyperlink ref="AB10" r:id="rId15" xr:uid="{0FC945F7-0BCC-40F4-B4E3-E6F894016718}"/>
+    <hyperlink ref="AB3" r:id="rId16" xr:uid="{892FEFC0-275E-4B58-BD6C-D9BDFE0D4683}"/>
+    <hyperlink ref="Z4" r:id="rId17" xr:uid="{E7F32542-A0E9-4257-B181-0F070656A46B}"/>
+    <hyperlink ref="Z5" r:id="rId18" location="box_eventlist" xr:uid="{C91DC913-B4BE-439E-A172-CABC5BD9135C}"/>
+    <hyperlink ref="Z6" r:id="rId19" location="box_eventlist" xr:uid="{67A1985E-7360-40D8-B1A5-0A0A8347F1F3}"/>
+    <hyperlink ref="Z7" r:id="rId20" location="box_eventlist" xr:uid="{F523150D-BBB4-4101-92F0-B403FD1E1E29}"/>
+    <hyperlink ref="Z8" r:id="rId21" location="box_eventlist" xr:uid="{65FC9304-735F-4591-8831-97A124A03080}"/>
+    <hyperlink ref="AB4" r:id="rId22" xr:uid="{BB033F2D-BA45-4EC2-BECD-C271083EA49F}"/>
+    <hyperlink ref="AB5" r:id="rId23" xr:uid="{80E71080-A796-482D-AFE8-057F9DD033C2}"/>
+    <hyperlink ref="AB6" r:id="rId24" xr:uid="{4216133B-27C6-4840-BBCB-2927320E7BB9}"/>
+    <hyperlink ref="AB7" r:id="rId25" xr:uid="{A33E7745-3088-4FC7-B9F6-334EAF876555}"/>
+    <hyperlink ref="AB8" r:id="rId26" xr:uid="{B7593B2F-2A95-4944-9B48-B5659E284681}"/>
+    <hyperlink ref="K4" r:id="rId27" xr:uid="{C3130B72-0165-4E90-8275-C0F9022E4C0E}"/>
+    <hyperlink ref="K5" r:id="rId28" location="box_eventlist" xr:uid="{957040E1-67C5-4C26-B28E-7B78E078A5B7}"/>
+    <hyperlink ref="K6" r:id="rId29" location="box_eventlist" xr:uid="{E9D9A156-D816-48E2-A815-401344FDB15B}"/>
+    <hyperlink ref="K7" r:id="rId30" location="box_eventlist" xr:uid="{B4B69F15-159A-4D92-A803-846AF90EDB5A}"/>
+    <hyperlink ref="K8" r:id="rId31" location="box_eventlist" xr:uid="{DFC53AA5-6BCF-4F4C-818C-223B1B6F83F4}"/>
+    <hyperlink ref="K11" r:id="rId32" xr:uid="{42F0FFF5-ECD4-4C5D-A6B2-1A2796827423}"/>
+    <hyperlink ref="L11" r:id="rId33" xr:uid="{906417F1-A115-42CA-9DB1-2AA6F270AF56}"/>
+    <hyperlink ref="AB11" r:id="rId34" xr:uid="{2B99C277-A524-44C4-959D-A259057E2DCF}"/>
+    <hyperlink ref="L13" r:id="rId35" xr:uid="{01120292-E8C0-424E-8346-241376FE0528}"/>
+    <hyperlink ref="L14" r:id="rId36" xr:uid="{CD05EDE3-8105-4C85-A64E-DB39DD3B1620}"/>
+    <hyperlink ref="K13" r:id="rId37" xr:uid="{B5D4D292-0041-4DEA-BE63-83D14D66EDDB}"/>
+    <hyperlink ref="K14" r:id="rId38" xr:uid="{87A2E6C2-43A2-48E0-8F5D-55926481A8FA}"/>
+    <hyperlink ref="V13" r:id="rId39" xr:uid="{5CF90B70-0399-4A08-A04C-285E4080E9BB}"/>
+    <hyperlink ref="V14" r:id="rId40" xr:uid="{57563E15-8C24-4A36-8605-01E183D2335C}"/>
+    <hyperlink ref="AB13" r:id="rId41" xr:uid="{E57EB0D7-F269-4C81-858F-424E1536E6FB}"/>
+    <hyperlink ref="AB14" r:id="rId42" xr:uid="{6EFD9474-17B2-407A-9635-9617C89A7061}"/>
+    <hyperlink ref="L16" r:id="rId43" location="box_eventlist" xr:uid="{C8D18862-2904-4DC9-BCD9-EF2E4CE8F840}"/>
+    <hyperlink ref="L15" r:id="rId44" xr:uid="{CF3A4B1E-6246-4153-BCA5-6DEA7CD8128F}"/>
+    <hyperlink ref="K16" r:id="rId45" location="box_eventlist" xr:uid="{B01E5353-4015-4146-9B14-1B1CCE53F5E5}"/>
+    <hyperlink ref="K15" r:id="rId46" xr:uid="{560D83FF-C50C-4694-8721-F77C0BFF08C5}"/>
+    <hyperlink ref="AB15" r:id="rId47" xr:uid="{4011499F-8062-43B8-A75C-A9079EF2DB52}"/>
+    <hyperlink ref="AB16" r:id="rId48" xr:uid="{B6B3C075-FA6C-467D-8AA6-1D1EED92C415}"/>
+    <hyperlink ref="V15" r:id="rId49" xr:uid="{A072C560-8B04-430B-B1F6-B028E5FA9574}"/>
+    <hyperlink ref="V16" r:id="rId50" xr:uid="{ACA9C9AF-B973-43C4-9DB4-EBC4EECAAE25}"/>
+    <hyperlink ref="AK9" r:id="rId51" xr:uid="{E1E89324-2E73-407A-A30A-BDBE667C6060}"/>
+    <hyperlink ref="AK3" r:id="rId52" xr:uid="{D29EF5FB-36E0-463F-8BF5-132FE5F9A756}"/>
+    <hyperlink ref="AK4:AK8" r:id="rId53" display="https://www.bfz.de/kontakt" xr:uid="{01FE9A2A-D98E-4C72-A768-E4E97D2D26C9}"/>
+    <hyperlink ref="AK10" r:id="rId54" xr:uid="{D3534D7D-125C-4937-A705-03B6F4680DED}"/>
+    <hyperlink ref="AK11" r:id="rId55" xr:uid="{3D21D631-AA2F-409E-9F5C-4559889C3D91}"/>
+    <hyperlink ref="AK12" r:id="rId56" xr:uid="{D9C7ECDE-18FC-4416-B929-BE0EAB7C5622}"/>
+    <hyperlink ref="AK13" r:id="rId57" xr:uid="{90BE5531-03FA-4904-8588-E71407AF76F4}"/>
+    <hyperlink ref="AK14" r:id="rId58" xr:uid="{4132C431-E473-45EF-83C8-DB75A0F0851B}"/>
+    <hyperlink ref="AK15" r:id="rId59" xr:uid="{967ECC8C-EFCA-431C-874F-910F1558F1C8}"/>
+    <hyperlink ref="AK16" r:id="rId60" xr:uid="{32AE002E-D17E-4E2A-B510-AA0C0E1F52E7}"/>
+    <hyperlink ref="AK17" r:id="rId61" xr:uid="{9B55CF75-F045-419D-A6A4-15C1B4651E38}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId62"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0a02612f-c061-4319-bfdb-b5863aa27d0a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100422B2238F8DAAD478C0837055D4C9439" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3cc5534cd780fd9e31c09b047b200ae0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8859808f-556d-416b-ba10-3a64d67cd7c4" xmlns:ns4="0a02612f-c061-4319-bfdb-b5863aa27d0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47912ec95e7c0f2f58d4b636259ebaea" ns3:_="" ns4:_="">
     <xsd:import namespace="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
@@ -2010,10 +4407,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0a02612f-c061-4319-bfdb-b5863aa27d0a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D77567D-EF8B-449E-AB9D-98DD6B7BC045}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7DC12C-AC0B-45A5-9CE7-33B2216F9746}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
+    <ds:schemaRef ds:uri="0a02612f-c061-4319-bfdb-b5863aa27d0a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2036,20 +4461,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7DC12C-AC0B-45A5-9CE7-33B2216F9746}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D77567D-EF8B-449E-AB9D-98DD6B7BC045}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
-    <ds:schemaRef ds:uri="0a02612f-c061-4319-bfdb-b5863aa27d0a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Usecase Data for december Testung according to feedback
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/UseCaseCourseData.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/UseCaseCourseData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74ED414-1786-44E7-B194-9CEB9796F007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58617604-EFF5-48A0-81F4-A02BFD00F766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17028" yWindow="4188" windowWidth="26112" windowHeight="17352" activeTab="1" xr2:uid="{42E46E1E-8980-4662-AB6D-571AD8C791C7}"/>
+    <workbookView xWindow="336" yWindow="5928" windowWidth="21588" windowHeight="17352" activeTab="1" xr2:uid="{42E46E1E-8980-4662-AB6D-571AD8C791C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="461">
   <si>
     <t>CourseProviderId</t>
   </si>
@@ -727,9 +727,6 @@
     <t>13.02.2023</t>
   </si>
   <si>
-    <t>07.06.2024</t>
-  </si>
-  <si>
     <t>https://www.bfz.de/kontakt</t>
   </si>
   <si>
@@ -1119,9 +1116,6 @@
     <t>beratung@bfz.de</t>
   </si>
   <si>
-    <t xml:space="preserve">Beratung </t>
-  </si>
-  <si>
     <t>19 Wochen</t>
   </si>
   <si>
@@ -1136,12 +1130,6 @@
   </si>
   <si>
     <t>Teilzeit, Vollzeit möglich https://www.bfz.de/kurs/eca-90154/pdf/90154-23-001-4/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1.pdf https://www.bfz.de/kurs/eca-90154/pdf/90154-23-003-4/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1.pdf</t>
-  </si>
-  <si>
-    <t>ismail.debre@bfz.de</t>
-  </si>
-  <si>
-    <t>Ismail Debre</t>
   </si>
   <si>
     <t>07.07.2023</t>
@@ -1775,12 +1763,171 @@
   <si>
     <t>AttendeeCertificate</t>
   </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>FullTimeAndPartTime</t>
+  </si>
+  <si>
+    <t>PostQualified</t>
+  </si>
+  <si>
+    <t>28.08.2023</t>
+  </si>
+  <si>
+    <t>Claudia von Lueder</t>
+  </si>
+  <si>
+    <t>qualifizierung-m@bfz.de</t>
+  </si>
+  <si>
+    <t>Monika Geisberger</t>
+  </si>
+  <si>
+    <t>+4989189552934</t>
+  </si>
+  <si>
+    <t>15.09.2023</t>
+  </si>
+  <si>
+    <t>https://www.bfz.de/kurs-kontakt/eca-90154/kaufmannfrau-im-e-commerce-warenwirtschaft-und-onlinevertrieb-modul-1/90154-23-001-4/kontakt</t>
+  </si>
+  <si>
+    <t>&lt;Label TextType=\"Html\"&gt;\r\n    
+&lt;![CDATA[\r\n        
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/1dd23dba-dd00-45ab-abf4-642902538317" target=\"_blank\"&gt;Risikoanalyse durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0ee94af1-b445-4973-9c3f-459fab250342" target=\"_blank\"&gt;Konfliktmanagement anwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/22902bf9-cc3f-495b-811a-c441e28e23f6" target=\"_blank\"&gt;Projektinformationen verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/496932f1-0b6b-4f73-9432-d95c7ddcd43b" target=\"_blank\"&gt;Mitarbeiter einstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/f5dd06b8-5d17-4932-9d03-957d0c4f5051" target=\"_blank\"&gt;Ressourcenplanung durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0cc9c234-f817-4f4c-908a-4d28fe3b0f4a" target=\"_blank\"&gt;Mitarbeiter/Mitarbeiterinnen coachen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/b9bf9e17-ae47-417b-bbb1-e8b7c263ccac" target=\"_blank\"&gt;rechtliche Bestimmungen ermitteln&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/4df7a57a-9405-4995-8e02-4ca404832247" target=\"_blank\"&gt;Projektänderungen verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/cd5efa8c-e44d-4cbc-91c6-796018dbed68" target=\"_blank\"&gt;Projekte managen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/3c76296d-4bbd-44ba-8eaa-95bf275f79b7" target=\"_blank\"&gt;IKT-Projekt leiten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/48b68726-0fd6-4e03-a5eb-82236516ee7a" target=\"_blank\"&gt;Berichte über Kosten-Nutzen-Analysen bereitstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/21fecc8a-392e-49ce-ac26-fb0696ccfead" target=\"_blank\"&gt;Projektspezifikationen erarbeiten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/339ac029-066a-4985-9f9d-b3d7c8fea0bb" target=\"_blank\"&gt;Mitarbeiter führen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/dc72ad0a-c5dc-4abd-bc0d-ca43e82162e1" target=\"_blank\"&gt;Geschäftsbeziehungen aufbauen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/21c5790c-0930-4d74-b3b0-84caf5af12ea" target=\"_blank\"&gt;Finanzmittel verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/e207163b-7963-4c3e-9494-7a4bb000211b" target=\"_blank\"&gt;voraussichtliche Dauer der Arbeiten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/e54ff029-1ce9-447d-a5b2-eb7283a23e6e" target=\"_blank\"&gt;Personal schulen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/8d4271ca-c9fd-40b3-875f-15f78332a49e" target=\"_blank\"&gt;Qualitätsstandards&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/bec4359e-cb92-468f-a997-8fb28e32fba9" target=\"_blank\"&gt;IKT-Projektmanagement-Methoden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0daaf096-1639-461c-bf1a-bbeea77e6b67" target=\"_blank\"&gt;Richtlinien des internen Risikomanagements&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/94dd823c-148e-4614-a6e8-99249b16357d" target=\"_blank\"&gt;IuK-Projektmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/c3687b34-fe53-4db2-ad1b-5055a6c5b6fd" target=\"_blank\"&gt;Projekttreffen organisieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/bc067d2e-e151-408f-8e34-24effd2b7fd6" target=\"_blank\"&gt;elektronische Beschaffung nutzen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/69cfc5ed-6569-4aca-a4cc-fd782ba51d9c" target=\"_blank\"&gt;IKT-Risikomanagement durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d9e5349e-8791-49c2-8ba4-839fdd1606c2" target=\"_blank\"&gt;technische Anforderungen definieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d3eccb86-f02d-4950-bfbd-20b9510774a1" target=\"_blank\"&gt;organisatorische Techniken anwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/a9bf8565-8a09-4118-9922-932d65a79d69" target=\"_blank\"&gt;Lokalisierung leiten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/7e1f9657-ab4e-407c-842f-b846197060e3" target=\"_blank\"&gt;IKT-Audits durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/f17f94f1-88cb-4815-873a-2a9639f10729" target=\"_blank\"&gt;Projektunterlagen ausarbeiten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/03b9b491-fc9b-4868-914a-bf7cd47b5041" target=\"_blank\"&gt;Problemlösungen finden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/770d4956-b5e0-4d44-bf42-3a766b232c5d" target=\"_blank\"&gt;ein zentrales Projekt-Repository unterhalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/3c03ee71-4a23-448f-b79e-81fd75d27dca" target=\"_blank\"&gt;Änderungsmanagement anwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/3cd35f5d-ce6d-4f14-9a09-53d7a28d834c" target=\"_blank\"&gt;Beziehungen zu Lieferanten pflegen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/9e9a4209-c7cf-4f6e-973e-dc2ffadccc74" target=\"_blank\"&gt;Beschaffungsprozesse durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6430eb0d-c6de-46b7-a7fc-3dd2e8e62a69" target=\"_blank\"&gt;IKT-Fallbearbeitungssystem verwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/04dfd9fb-e0cf-40f6-96c6-9d2280c4347e" target=\"_blank\"&gt;technische Dokumentation bereitstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/1b3fc0e0-c6f9-45fc-9c6e-14bbba662979" target=\"_blank\"&gt;Informationsnormen entwickeln&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/1fcce318-3212-487a-ac07-4941bc85060d" target=\"_blank\"&gt;Projektaktivitäten durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/96eb286a-58b7-45ff-a916-5578d0b79b8c" target=\"_blank\"&gt;Rapid Application Development&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ed1d8bd4-cd2a-4c64-b665-56d70651026c" target=\"_blank\"&gt;Prototyping&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/eff1bb34-b454-4482-8c29-65f820619f3c" target=\"_blank\"&gt;Insourcing-Strategie&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/a846cb9e-c152-41e7-bd34-45e7ff941e3b" target=\"_blank\"&gt;gesetzliche Vorschriften für IuK-Produkte&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/fafe0b9d-dbd9-46bd-b770-26299539ce66" target=\"_blank\"&gt;Qualitätsmodelle für ITK-Prozesse&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ccb2e5f2-4279-48fd-9d85-a1db42ff1e13" target=\"_blank\"&gt;Projekt-Konfigurationsmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/c7cc6dc5-d56b-4323-8e5c-47c4022f615f" target=\"_blank\"&gt;Verfahren der Qualitätssicherung&lt;/a&gt;.\r\n\t
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/b16200f4-4f39-4b8b-aa9d-3568054d6bdb" target=\"_blank\"&gt;Open-Source-Modell&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/da6393d5-a53c-4863-abc7-51f36281d74e" target=\"_blank\"&gt;schlankes Projektmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/dba46f87-0831-49cd-a1c7-340a653c0221" target=\"_blank\"&gt;agile Entwicklung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/8ff015a0-98ea-4d80-a23e-1f68110a919e" target=\"_blank\"&gt;Softwareentwicklungsmethoden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/694dc996-52f3-4afa-a802-672e19f061b7" target=\"_blank\"&gt;Crowdsourcing-Strategie&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/00c04e40-35ea-4ed1-824c-82f936c8f876" target=\"_blank\"&gt;inkrementelle Entwicklung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/67a118f4-8a5f-48f7-8e5f-de34b9ca2c37" target=\"_blank\"&gt;Hybridmodell&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/2450c3b3-e78e-435b-b84d-e05d984e71dc" target=\"_blank\"&gt;Softwarearchitekturmodelle&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6f8baa62-bc2b-4cc1-942b-f540c837cfa2" target=\"_blank\"&gt;Outsourcing-Strategie&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ca73ac82-867a-4afa-9732-834aebe896ff" target=\"_blank\"&gt;Nutzeranforderungen an das IKT-System&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6a876489-7ad8-4a13-b09c-c9b8e97a302e" target=\"_blank\"&gt;Wasserfallmodell&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/33d49d4f-31ec-473f-9b8a-b555aa5116bb" target=\"_blank\"&gt;iterative Entwicklung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/83218cac-3599-417e-93d2-26013cdccd98" target=\"_blank\"&gt;serviceorientierte Modellierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/4840338b-ac6c-486a-be1d-9ddfe00b8bdf" target=\"_blank\"&gt;Spiralmodell&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0a9acb6b-1139-4be9-b431-3a80a959f2f4" target=\"_blank\"&gt;agiles Projektmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/eeca3780-8049-499f-a268-95a7ad26642c" target=\"_blank\"&gt;SaaS-Modell&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/09f2f811-a3fb-4de3-a70f-6420a6935575" target=\"_blank\"&gt;Systementwicklungszyklus&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/f0de4973-0a70-4644-8fd4-3a97080476f4" target=\"_blank\"&gt;DevOps&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/5be3d306-6cf1-4b49-aa1d-01651dd4ba4c" target=\"_blank\"&gt;objektorientierte Modellierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ea1bf5e5-e7f0-4d2c-a415-1c39c00512b1" target=\"_blank\"&gt;IuK-Dokumentenmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d5a59ca8-2e91-472e-8571-d12ce4478679" target=\"_blank\"&gt;prozessorientiertes Management&lt;/a&gt;.\r\n\t 
+]]&gt;\r\n 
+&lt;/Label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Label TextType=\"Html\"&gt;\r\n    
+&lt;![CDATA[\r\n        
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/21d2f96d-35f7-4e3f-9745-c533d2dd6e97" target=\"_blank\"&gt;Computerprogrammierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/14d1e367-3efe-4ec5-86ae-eca48710ee4e" target=\"_blank\"&gt;IKT-Sicherheitsstrategie umsetzen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0dc7aa1b-b5af-4f4b-81ce-ee22ed8b6926" target=\"_blank\"&gt;IKT-Kenntnisse bewerten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/29fb0fb5-dfc4-4098-ac9b-3a712000f48f" target=\"_blank\"&gt;Datenbank verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d9e5349e-8791-49c2-8ba4-839fdd1606c2" target=\"_blank\"&gt;technische Anforderungen definieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0af062de-eb43-41e9-9b96-249e2cd22d26" target=\"_blank\"&gt;Auszeichnungssprachen verwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/fbafa41f-cd05-4109-a649-8b44d306d779" target=\"_blank\"&gt;Datenmodelle erstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/b04f377b-ee80-4b38-aca1-19d266a23b17" target=\"_blank\"&gt;Anforderungen der Geschäftswelt analysieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ed8de897-adbe-4f0e-b4d2-534953e64c72 target=\"_blank\"&gt;Systemkomponenten integrieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/2857540c-180b-4208-9127-e94a01871966" target=\"_blank\"&gt;Software an Systemarchitekturen anpassen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/04fe962b-4017-4eb7-9139-7d69b6922bc9" target=\"_blank\"&gt;anwendungsspezifische Schnittstelle verwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ee3c1d54-f46a-43c7-a0f9-0ba3648164d0" target=\"_blank\"&gt;Unternehmensarchitektur konzipieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/cbe2c304-1e7d-489a-97d9-a7d3e37a9db6" target=\"_blank\"&gt;IKT-Systemtheorie anwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/ce354460-500e-4eaa-8e95-8f243fcea3db" target=\"_blank\"&gt;Systemtests durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/69bbd53f-fbb0-4476-b4b2-ef7844464e28" target=\"_blank\"&gt;Webprogrammierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/117373c8-f04b-4fff-8683-aebe36edac81" target=\"_blank\"&gt;Hardwareplattformen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/09f2f811-a3fb-4de3-a70f-6420a6935575" target=\"_blank\"&gt;Systementwicklungszyklus&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/cdd8b6b2-2fd9-453c-8d62-8a1dc6efcd49" target=\"_blank\"&gt;Systemtheorie&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/9ef0f3a0-9ce2-4ef1-a987-0366b5cb2dbe" target=\"_blank\"&gt;Datenbank-Entwicklungswerkzeuge&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/98301d4a-2cc3-439d-8d7f-0b6ac76302bb" target=\"_blank\"&gt;Geschäftsprozessmodellierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/339ac029-066a-4985-9f9d-b3d7c8fea0bb" target=\"_blank\"&gt;Mitarbeiter führen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/9e06bac6-6b91-48ca-8b7d-c1f48cdecd7c" target=\"_blank\"&gt;IKT-Systemprobleme lösen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/dfff95c6-9758-4c04-a228-7eaa88dec6cd" target=\"_blank\"&gt;organisatorische Komplexität bei der Planung berücksichtigen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/11430d93-c835-48ed-8e70-285fa69c9ae6" target=\"_blank\"&gt;Cloud-Architektur konzipieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/04dfd9fb-e0cf-40f6-96c6-9d2280c4347e" target=\"_blank\"&gt;technische Dokumentation bereitstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0a52bed5-fd29-45fb-aba6-e32bccfda1c1" target=\"_blank\"&gt;Migration in die Cloud planen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/5b9cde20-f1b9-4adc-bfb3-dbf70b14138d" target=\"_blank\"&gt;objektorientierte Programmierung verwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/f5dd06b8-5d17-4932-9d03-957d0c4f5051" target=\"_blank\"&gt;Ressourcenplanung durchführen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/7e796b51-49d7-4e73-95af-2e7323763f15" target=\"_blank\"&gt;Datenbank in der Cloud konzipieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6c08403c-a5bb-4868-b8c2-b7d039c0e511" target=\"_blank\"&gt;Datenbankschema konzipieren&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/cb5cccc9-abe4-4b11-abe6-d27e5cd85fb1" target=\"_blank\"&gt;Standards für den Datenaustausch verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/c32ad607-0c4d-4e34-b73f-668298f7bf13" target=\"_blank\"&gt;Fähigkeiten zur Kommunikation über Technik anwenden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d3286405-49f8-4e8a-8046-a4376b4e7963" target=\"_blank\"&gt;Cloud-Daten und -Speicher verwalten&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6b643893-0a1f-4f6c-83a1-e7eef75849b9" target=\"_blank\"&gt;Code mit Cloud-Diensten schreiben&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/2c28fc20-8a60-4311-8899-5ef8729c05b3" target=\"_blank\"&gt;Gestaltungsprozess&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/dc72ad0a-c5dc-4abd-bc0d-ca43e82162e1" target=\"_blank\"&gt;Geschäftsbeziehungen aufbauen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/48b68726-0fd6-4e03-a5eb-82236516ee7a" target=\"_blank\"&gt;Berichte über Kosten-Nutzen-Analysen bereitstellen&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/0a9acb6b-1139-4be9-b431-3a80a959f2f4" target=\"_blank\"&gt;agiles Projektmanagement&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/d5a59ca8-2e91-472e-8571-d12ce4478679" target=\"_blank\"&gt;prozessorientiertes Management&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/25df422a-bf0a-4f76-8631-d0be91cb8751" target=\"_blank\"&gt;modellbasierte Systemtechnik&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/7482a123-e801-48de-9733-262125671410" target=\"_blank\"&gt;Aufgaben-Algorithmisierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/17924c75-45f4-4593-afac-eea0d51f04b5" target=\"_blank\"&gt;Standardverfahren der Verteidigung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/7814e88f-c133-4c3b-b27f-857afa145d42" target=\"_blank\"&gt;IKT-Sicherheitsgesetzgebung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/fafe0b9d-dbd9-46bd-b770-26299539ce66" target=\"_blank\"&gt;Qualitätsmodelle für ITK-Prozesse&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/bec4359e-cb92-468f-a997-8fb28e32fba9" target=\"_blank\"&gt;IKT-Projektmanagement-Methoden&lt;/a&gt;.\r\n\t
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/6fa1c2c0-a012-4ca0-9642-e01569ba322c" target=\"_blank\"&gt;IKT-Systemintegration&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/a4d336a6-9ffd-402a-91cc-f359716ba4e0" target=\"_blank\"&gt;ML (Computerprogrammierung)&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/03ff0d53-573a-47a0-a0ad-1995815a4339" target=\"_blank\"&gt;Informationsstruktur&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/8ff015a0-98ea-4d80-a23e-1f68110a919e" target=\"_blank\"&gt;Softwareentwicklungsmethoden&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/b105ec9b-0857-41d6-8d07-a83e58b73d90" target=\"_blank\"&gt;IKT-Systemprogrammierung&lt;/a&gt;.\r\n\t 
+&lt;a href=\"https://esco.ec.europa.eu/de/classification/skills?uri=http://data.europa.eu/esco/skill/da6393d5-a53c-4863-abc7-51f36281d74e" target=\"_blank\"&gt;schlankes Projektmanagement&lt;/a&gt;.\r\n\t 
+]]&gt;\r\n 
+&lt;/Label&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1894,8 +2041,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="MesloLGM NF"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1941,6 +2094,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1993,7 +2152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2076,6 +2235,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2664,7 +2826,7 @@
         <v>5</v>
       </c>
       <c r="BI2" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ2" s="7" t="s">
         <v>112</v>
@@ -2732,7 +2894,7 @@
         <v>5</v>
       </c>
       <c r="BI3" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ3" s="7" t="s">
         <v>112</v>
@@ -2800,7 +2962,7 @@
         <v>5</v>
       </c>
       <c r="BI4" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ4" s="7" t="s">
         <v>112</v>
@@ -2868,7 +3030,7 @@
         <v>5</v>
       </c>
       <c r="BI5" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ5" s="7" t="s">
         <v>112</v>
@@ -2936,7 +3098,7 @@
         <v>5</v>
       </c>
       <c r="BI6" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ6" s="7" t="s">
         <v>112</v>
@@ -3004,7 +3166,7 @@
         <v>5</v>
       </c>
       <c r="BI7" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ7" s="7" t="s">
         <v>112</v>
@@ -3078,7 +3240,7 @@
         <v>5</v>
       </c>
       <c r="BI8" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ8" s="7" t="s">
         <v>112</v>
@@ -3149,7 +3311,7 @@
         <v>5</v>
       </c>
       <c r="BI9" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ9" s="7" t="s">
         <v>112</v>
@@ -3220,7 +3382,7 @@
         <v>5</v>
       </c>
       <c r="BI10" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ10" s="7" t="s">
         <v>112</v>
@@ -3291,7 +3453,7 @@
         <v>5</v>
       </c>
       <c r="BI11" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ11" s="7" t="s">
         <v>112</v>
@@ -3359,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="BI12" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ12" s="7" t="s">
         <v>112</v>
@@ -3427,7 +3589,7 @@
         <v>5</v>
       </c>
       <c r="BI13" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ13" s="7" t="s">
         <v>112</v>
@@ -3495,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="BI14" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ14" s="7" t="s">
         <v>112</v>
@@ -3564,7 +3726,7 @@
         <v>5</v>
       </c>
       <c r="BI15" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ15" s="12" t="s">
         <v>112</v>
@@ -3633,7 +3795,7 @@
         <v>5</v>
       </c>
       <c r="BI16" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ16" s="12" t="s">
         <v>112</v>
@@ -3702,7 +3864,7 @@
         <v>5</v>
       </c>
       <c r="BI17" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ17" s="12" t="s">
         <v>112</v>
@@ -3771,7 +3933,7 @@
         <v>5</v>
       </c>
       <c r="BI18" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ18" s="12" t="s">
         <v>112</v>
@@ -3840,7 +4002,7 @@
         <v>5</v>
       </c>
       <c r="BI19" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ19" s="12" t="s">
         <v>112</v>
@@ -3908,7 +4070,7 @@
         <v>5</v>
       </c>
       <c r="BI20" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ20" s="12" t="s">
         <v>112</v>
@@ -3979,7 +4141,7 @@
         <v>5</v>
       </c>
       <c r="BI21" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ21" s="12" t="s">
         <v>112</v>
@@ -4047,7 +4209,7 @@
         <v>5</v>
       </c>
       <c r="BI22" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ22" s="12" t="s">
         <v>112</v>
@@ -4115,7 +4277,7 @@
         <v>5</v>
       </c>
       <c r="BI23" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ23" s="12" t="s">
         <v>112</v>
@@ -4183,7 +4345,7 @@
         <v>5</v>
       </c>
       <c r="BI24" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ24" s="12" t="s">
         <v>112</v>
@@ -4251,7 +4413,7 @@
         <v>5</v>
       </c>
       <c r="BI25" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ25" s="12" t="s">
         <v>112</v>
@@ -4319,7 +4481,7 @@
         <v>5</v>
       </c>
       <c r="BI26" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ26" s="12" t="s">
         <v>112</v>
@@ -4387,7 +4549,7 @@
         <v>5</v>
       </c>
       <c r="BI27" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ27" s="12" t="s">
         <v>112</v>
@@ -4456,7 +4618,7 @@
         <v>5</v>
       </c>
       <c r="BI28" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ28" s="16" t="s">
         <v>112</v>
@@ -4525,7 +4687,7 @@
         <v>5</v>
       </c>
       <c r="BI29" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ29" s="16" t="s">
         <v>112</v>
@@ -4594,7 +4756,7 @@
         <v>5</v>
       </c>
       <c r="BI30" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ30" s="16" t="s">
         <v>112</v>
@@ -4663,7 +4825,7 @@
         <v>5</v>
       </c>
       <c r="BI31" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ31" s="16" t="s">
         <v>112</v>
@@ -4732,7 +4894,7 @@
         <v>5</v>
       </c>
       <c r="BI32" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ32" s="16" t="s">
         <v>112</v>
@@ -4800,7 +4962,7 @@
         <v>5</v>
       </c>
       <c r="BI33" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ33" s="16" t="s">
         <v>112</v>
@@ -4871,7 +5033,7 @@
         <v>5</v>
       </c>
       <c r="BI34" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ34" s="16" t="s">
         <v>112</v>
@@ -4939,7 +5101,7 @@
         <v>5</v>
       </c>
       <c r="BI35" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ35" s="16" t="s">
         <v>112</v>
@@ -5007,7 +5169,7 @@
         <v>5</v>
       </c>
       <c r="BI36" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ36" s="16" t="s">
         <v>112</v>
@@ -5075,7 +5237,7 @@
         <v>5</v>
       </c>
       <c r="BI37" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ37" s="16" t="s">
         <v>112</v>
@@ -5143,7 +5305,7 @@
         <v>5</v>
       </c>
       <c r="BI38" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ38" s="16" t="s">
         <v>112</v>
@@ -5211,7 +5373,7 @@
         <v>5</v>
       </c>
       <c r="BI39" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ39" s="16" t="s">
         <v>112</v>
@@ -5279,7 +5441,7 @@
         <v>5</v>
       </c>
       <c r="BI40" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="BJ40" s="16" t="s">
         <v>112</v>
@@ -5308,8 +5470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D671E26-080C-462D-901A-35D8ED7721D2}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5327,11 +5489,13 @@
     <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.88671875" customWidth="1"/>
+    <col min="15" max="15" width="43.44140625" customWidth="1"/>
     <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.35">
@@ -5507,7 +5671,7 @@
         <v>179</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
@@ -5527,7 +5691,7 @@
         <v>220</v>
       </c>
       <c r="AF2" s="25" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="AK2" s="1" t="s">
         <v>183</v>
@@ -5596,7 +5760,7 @@
         <v>179</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
@@ -5616,7 +5780,7 @@
         <v>220</v>
       </c>
       <c r="AF3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>183</v>
@@ -5685,7 +5849,7 @@
         <v>179</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
@@ -5702,10 +5866,10 @@
         <v>182</v>
       </c>
       <c r="AE4" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF4" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AK4" s="1" t="s">
         <v>183</v>
@@ -5774,7 +5938,7 @@
         <v>179</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
@@ -5791,10 +5955,10 @@
         <v>182</v>
       </c>
       <c r="AE5" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF5" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="AK5" s="1" t="s">
         <v>183</v>
@@ -5863,7 +6027,7 @@
         <v>179</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
@@ -5880,10 +6044,10 @@
         <v>182</v>
       </c>
       <c r="AE6" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AF6" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AK6" s="1" t="s">
         <v>183</v>
@@ -5952,7 +6116,7 @@
         <v>179</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
@@ -5969,16 +6133,16 @@
         <v>182</v>
       </c>
       <c r="AE7" s="25" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="AF7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="AG7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AH7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="AK7" s="1" t="s">
         <v>183</v>
@@ -6047,7 +6211,7 @@
         <v>179</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
@@ -6064,16 +6228,16 @@
         <v>182</v>
       </c>
       <c r="AE8" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF8" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AG8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AH8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AK8" s="1" t="s">
         <v>183</v>
@@ -6139,7 +6303,7 @@
         <v>215</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y9" s="7" t="s">
         <v>216</v>
@@ -6161,10 +6325,10 @@
         <v>220</v>
       </c>
       <c r="AF9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK9" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="AK9" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6199,44 +6363,44 @@
         <v>185</v>
       </c>
       <c r="K10" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="M10" t="s">
         <v>172</v>
       </c>
       <c r="N10" t="s">
+        <v>224</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" t="s">
         <v>211</v>
       </c>
       <c r="R10" t="s">
+        <v>226</v>
+      </c>
+      <c r="S10" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>215</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y10" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z10" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA10">
         <v>101</v>
@@ -6254,10 +6418,10 @@
         <v>220</v>
       </c>
       <c r="AF10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6289,47 +6453,47 @@
         <v>169</v>
       </c>
       <c r="J11" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="L11" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="M11" t="s">
         <v>172</v>
       </c>
       <c r="N11" t="s">
+        <v>234</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" t="s">
         <v>211</v>
       </c>
       <c r="R11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>215</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y11" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z11" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AA11">
         <v>101</v>
@@ -6344,13 +6508,13 @@
         <v>219</v>
       </c>
       <c r="AE11" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF11" t="s">
         <v>239</v>
       </c>
-      <c r="AF11" t="s">
-        <v>240</v>
-      </c>
       <c r="AK11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6382,47 +6546,47 @@
         <v>169</v>
       </c>
       <c r="J12" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="L12" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="M12" t="s">
         <v>172</v>
       </c>
       <c r="N12" t="s">
+        <v>243</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" t="s">
         <v>211</v>
       </c>
       <c r="R12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>215</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y12" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z12" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AA12">
         <v>101</v>
@@ -6437,13 +6601,19 @@
         <v>219</v>
       </c>
       <c r="AE12" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF12" t="s">
         <v>246</v>
       </c>
-      <c r="AF12" t="s">
-        <v>247</v>
+      <c r="AG12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>264</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6475,45 +6645,45 @@
         <v>169</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K13" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="M13" t="s">
         <v>172</v>
       </c>
       <c r="N13" t="s">
+        <v>249</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s">
         <v>211</v>
       </c>
       <c r="R13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>215</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA13">
         <v>101</v>
@@ -6528,19 +6698,19 @@
         <v>219</v>
       </c>
       <c r="AE13" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF13" t="s">
         <v>253</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>254</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>255</v>
       </c>
-      <c r="AH13" t="s">
-        <v>256</v>
-      </c>
       <c r="AK13" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6572,45 +6742,45 @@
         <v>169</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K14" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="M14" t="s">
         <v>172</v>
       </c>
       <c r="N14" t="s">
+        <v>258</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s">
         <v>211</v>
       </c>
       <c r="R14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>215</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y14" s="7"/>
       <c r="Z14" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AA14">
         <v>101</v>
@@ -6625,19 +6795,13 @@
         <v>219</v>
       </c>
       <c r="AE14" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF14" t="s">
         <v>262</v>
       </c>
-      <c r="AF14" t="s">
-        <v>263</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>264</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>265</v>
-      </c>
       <c r="AK14" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6656,74 +6820,74 @@
       <c r="F15" t="s">
         <v>205</v>
       </c>
-      <c r="G15" s="24" t="s">
-        <v>167</v>
+      <c r="G15" s="47" t="s">
+        <v>451</v>
       </c>
       <c r="H15" t="s">
+        <v>265</v>
+      </c>
+      <c r="I15" t="s">
+        <v>369</v>
+      </c>
+      <c r="J15" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="I15" t="s">
-        <v>169</v>
-      </c>
-      <c r="J15" s="24" t="s">
+      <c r="K15" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="L15" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M15" t="s">
         <v>172</v>
       </c>
       <c r="N15" t="s">
+        <v>268</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" t="s">
+        <v>270</v>
+      </c>
+      <c r="R15" t="s">
         <v>271</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="S15" s="26" t="s">
+      <c r="T15" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="T15" s="26" t="s">
+      <c r="U15" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="V15" s="27" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X15" s="28">
         <v>2880</v>
       </c>
       <c r="Y15" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15">
         <v>102</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC15" t="s">
         <v>277</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" s="25" t="s">
         <v>278</v>
-      </c>
-      <c r="AD15" s="25" t="s">
-        <v>279</v>
       </c>
       <c r="AE15" s="25"/>
       <c r="AK15" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6734,13 +6898,13 @@
         <v>200</v>
       </c>
       <c r="D16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>167</v>
@@ -6752,69 +6916,69 @@
         <v>169</v>
       </c>
       <c r="J16" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="L16" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M16" t="s">
         <v>172</v>
       </c>
       <c r="N16" t="s">
+        <v>283</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="R16" t="s">
         <v>286</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="T16" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="V16" s="27" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X16" s="28">
         <v>1547</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Z16" s="11"/>
       <c r="AA16">
         <v>201</v>
       </c>
       <c r="AB16" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC16" t="s">
         <v>290</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="AD16" s="25" t="s">
+      <c r="AE16" t="s">
         <v>292</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AF16" t="s">
         <v>293</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AG16" t="s">
         <v>294</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AH16" t="s">
         <v>295</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AK16" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="AK16" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6825,81 +6989,81 @@
         <v>202</v>
       </c>
       <c r="D17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I17" t="s">
         <v>169</v>
       </c>
       <c r="J17" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M17" t="s">
         <v>172</v>
       </c>
       <c r="N17" t="s">
+        <v>300</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="R17" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R17" s="29" t="s">
+      <c r="S17" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="T17" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U17" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V17" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X17" s="28">
         <v>2245</v>
       </c>
       <c r="Y17" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Z17" s="7"/>
       <c r="AA17" s="31">
         <v>201</v>
       </c>
       <c r="AB17" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC17" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC17" s="31" t="s">
+      <c r="AD17" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD17" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE17" s="25"/>
       <c r="AK17" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6913,56 +7077,56 @@
         <v>184</v>
       </c>
       <c r="D18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I18" t="s">
         <v>169</v>
       </c>
       <c r="J18" s="24"/>
       <c r="K18" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M18" t="s">
         <v>172</v>
       </c>
       <c r="N18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O18" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="R18" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R18" s="29" t="s">
+      <c r="S18" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U18" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V18" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="X18" s="28"/>
       <c r="Y18" s="30"/>
@@ -6971,17 +7135,17 @@
         <v>201</v>
       </c>
       <c r="AB18" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC18" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC18" s="31" t="s">
+      <c r="AD18" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD18" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE18" s="25"/>
       <c r="AK18" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6995,56 +7159,56 @@
         <v>184</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I19" t="s">
         <v>169</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M19" t="s">
         <v>172</v>
       </c>
       <c r="N19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="R19" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R19" s="29" t="s">
+      <c r="S19" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U19" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V19" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="X19" s="28"/>
       <c r="Y19" s="30"/>
@@ -7053,17 +7217,17 @@
         <v>201</v>
       </c>
       <c r="AB19" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC19" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC19" s="31" t="s">
+      <c r="AD19" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD19" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE19" s="25"/>
       <c r="AK19" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7077,56 +7241,56 @@
         <v>184</v>
       </c>
       <c r="D20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I20" t="s">
         <v>169</v>
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M20" t="s">
         <v>172</v>
       </c>
       <c r="N20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O20" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="R20" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R20" s="29" t="s">
+      <c r="S20" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="T20" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="U20" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U20" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V20" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X20" s="28"/>
       <c r="Y20" s="30"/>
@@ -7135,17 +7299,17 @@
         <v>201</v>
       </c>
       <c r="AB20" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC20" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC20" s="31" t="s">
+      <c r="AD20" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD20" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE20" s="25"/>
       <c r="AK20" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7159,56 +7323,56 @@
         <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I21" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="24"/>
       <c r="K21" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M21" t="s">
         <v>172</v>
       </c>
       <c r="N21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O21" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="R21" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R21" s="29" t="s">
+      <c r="S21" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U21" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V21" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X21" s="28"/>
       <c r="Y21" s="30"/>
@@ -7217,17 +7381,17 @@
         <v>201</v>
       </c>
       <c r="AB21" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC21" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC21" s="31" t="s">
+      <c r="AD21" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD21" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE21" s="25"/>
       <c r="AK21" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7241,56 +7405,56 @@
         <v>184</v>
       </c>
       <c r="D22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>167</v>
       </c>
       <c r="H22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I22" t="s">
         <v>169</v>
       </c>
       <c r="J22" s="24"/>
       <c r="K22" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M22" t="s">
         <v>172</v>
       </c>
       <c r="N22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O22" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q22" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="R22" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="R22" s="29" t="s">
+      <c r="S22" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="T22" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U22" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="V22" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="X22" s="28"/>
       <c r="Y22" s="30"/>
@@ -7299,17 +7463,17 @@
         <v>201</v>
       </c>
       <c r="AB22" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC22" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC22" s="31" t="s">
+      <c r="AD22" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="AD22" s="33" t="s">
-        <v>292</v>
       </c>
       <c r="AE22" s="25"/>
       <c r="AK22" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:37" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7329,7 +7493,7 @@
         <v>166</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H23" s="34" t="s">
         <v>206</v>
@@ -7338,31 +7502,31 @@
         <v>169</v>
       </c>
       <c r="J23" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="K23" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="K23" s="36" t="s">
-        <v>320</v>
-      </c>
       <c r="L23" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M23" s="34" t="s">
         <v>172</v>
       </c>
       <c r="N23" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="O23" s="37" t="s">
         <v>321</v>
-      </c>
-      <c r="O23" s="37" t="s">
-        <v>322</v>
       </c>
       <c r="Q23" s="34" t="s">
         <v>175</v>
       </c>
       <c r="R23" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="S23" s="34" t="s">
         <v>323</v>
-      </c>
-      <c r="S23" s="34" t="s">
-        <v>324</v>
       </c>
       <c r="T23" s="34" t="s">
         <v>178</v>
@@ -7371,26 +7535,26 @@
         <v>179</v>
       </c>
       <c r="V23" s="45" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="X23" s="28"/>
       <c r="AA23" s="34">
         <v>30</v>
       </c>
       <c r="AB23" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC23" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="AC23" s="34" t="s">
+      <c r="AD23" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="AD23" s="39" t="s">
-        <v>327</v>
-      </c>
       <c r="AE23" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF23" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AK23" s="38" t="s">
         <v>183</v>
@@ -7416,7 +7580,7 @@
         <v>166</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H24" s="40" t="s">
         <v>206</v>
@@ -7425,31 +7589,31 @@
         <v>169</v>
       </c>
       <c r="J24" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="K24" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="L24" s="38" t="s">
         <v>328</v>
-      </c>
-      <c r="K24" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="L24" s="38" t="s">
-        <v>329</v>
       </c>
       <c r="M24" s="40" t="s">
         <v>172</v>
       </c>
       <c r="N24" s="40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O24" s="42" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q24" s="40" t="s">
         <v>175</v>
       </c>
       <c r="R24" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="S24" s="40" t="s">
         <v>323</v>
-      </c>
-      <c r="S24" s="40" t="s">
-        <v>324</v>
       </c>
       <c r="T24" s="40" t="s">
         <v>178</v>
@@ -7458,26 +7622,26 @@
         <v>179</v>
       </c>
       <c r="V24" s="46" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="X24" s="28"/>
       <c r="AA24" s="40">
         <v>30</v>
       </c>
       <c r="AB24" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC24" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="AC24" s="40" t="s">
+      <c r="AD24" s="43" t="s">
         <v>326</v>
       </c>
-      <c r="AD24" s="43" t="s">
-        <v>327</v>
-      </c>
       <c r="AE24" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF24" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AK24" s="38" t="s">
         <v>183</v>
@@ -7500,7 +7664,7 @@
         <v>205</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H25" t="s">
         <v>206</v>
@@ -7509,31 +7673,31 @@
         <v>169</v>
       </c>
       <c r="J25" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M25" t="s">
         <v>172</v>
       </c>
       <c r="N25" t="s">
+        <v>332</v>
+      </c>
+      <c r="O25" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="Q25" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="R25" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="R25" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="S25" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>178</v>
@@ -7542,7 +7706,7 @@
         <v>215</v>
       </c>
       <c r="V25" s="46" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="X25" s="28"/>
       <c r="Y25" s="7"/>
@@ -7551,15 +7715,15 @@
         <v>130</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AC25" s="31" t="s">
-        <v>338</v>
+        <v>453</v>
       </c>
       <c r="AD25" s="25"/>
       <c r="AE25" s="25"/>
       <c r="AK25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7579,40 +7743,40 @@
         <v>205</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H26" t="s">
         <v>206</v>
       </c>
       <c r="I26" t="s">
-        <v>169</v>
+        <v>450</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M26" t="s">
         <v>172</v>
       </c>
       <c r="N26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q26" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="R26" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="R26" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="S26" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>178</v>
@@ -7621,31 +7785,39 @@
         <v>215</v>
       </c>
       <c r="V26" s="46" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="X26" s="28"/>
       <c r="Y26" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="Z26" s="7"/>
       <c r="AA26">
         <v>130</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>344</v>
+        <v>454</v>
       </c>
       <c r="AC26" t="s">
-        <v>345</v>
-      </c>
-      <c r="AD26" s="25"/>
+        <v>455</v>
+      </c>
+      <c r="AD26" s="25" t="s">
+        <v>456</v>
+      </c>
       <c r="AE26" s="25" t="s">
         <v>220</v>
       </c>
       <c r="AF26" t="s">
-        <v>346</v>
+        <v>342</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>457</v>
       </c>
       <c r="AK26" s="1" t="s">
-        <v>222</v>
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7656,16 +7828,16 @@
         <v>230</v>
       </c>
       <c r="D27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H27" t="s">
         <v>206</v>
@@ -7674,66 +7846,66 @@
         <v>169</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="M27" t="s">
         <v>172</v>
       </c>
       <c r="N27" t="s">
+        <v>345</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="R27" t="s">
+        <v>348</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="T27" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="Q27" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="R27" t="s">
-        <v>352</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="V27" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="X27" s="28"/>
       <c r="Y27" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Z27" s="7"/>
       <c r="AA27">
         <v>201</v>
       </c>
       <c r="AB27" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC27" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AD27" s="25" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AE27" s="25" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AF27" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AK27" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -7753,7 +7925,7 @@
         <v>166</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H28" t="s">
         <v>206</v>
@@ -7762,37 +7934,37 @@
         <v>169</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="M28" t="s">
         <v>172</v>
       </c>
       <c r="N28" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="R28" t="s">
+        <v>286</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="T28" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="R28" t="s">
-        <v>287</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="T28" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="V28" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="X28" s="28">
         <v>1635</v>
@@ -7803,28 +7975,28 @@
         <v>61</v>
       </c>
       <c r="AB28" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>364</v>
+      </c>
+      <c r="AD28" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE28" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>294</v>
+      </c>
+      <c r="AH28" t="s">
         <v>367</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="AK28" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="AD28" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="AE28" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>370</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>295</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>371</v>
-      </c>
-      <c r="AK28" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -7844,46 +8016,43 @@
         <v>205</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>451</v>
-      </c>
-      <c r="H29" t="s">
-        <v>298</v>
+        <v>449</v>
       </c>
       <c r="I29" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="M29" t="s">
         <v>172</v>
       </c>
       <c r="N29" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q29" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="T29" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="Q29" s="11" t="s">
+      <c r="U29" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="T29" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="X29" s="28">
         <v>5900</v>
@@ -7894,22 +8063,22 @@
         <v>160</v>
       </c>
       <c r="AB29" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>380</v>
+      </c>
+      <c r="AD29" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE29" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="AF29" t="s">
         <v>383</v>
       </c>
-      <c r="AC29" t="s">
+      <c r="AK29" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="AD29" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="AE29" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>387</v>
-      </c>
-      <c r="AK29" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -7929,40 +8098,40 @@
         <v>205</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="H30" t="s">
         <v>206</v>
       </c>
       <c r="I30" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="M30" t="s">
         <v>172</v>
       </c>
       <c r="N30" s="44" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="T30" s="2"/>
       <c r="X30" s="28"/>
@@ -7972,22 +8141,22 @@
         <v>160</v>
       </c>
       <c r="AB30" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AC30" t="s">
+        <v>380</v>
+      </c>
+      <c r="AD30" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE30" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>392</v>
+      </c>
+      <c r="AK30" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="AD30" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="AE30" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>396</v>
-      </c>
-      <c r="AK30" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
@@ -8007,44 +8176,44 @@
         <v>205</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I31" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="M31" t="s">
         <v>172</v>
       </c>
       <c r="N31" s="44" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="X31" s="28">
         <v>2400</v>
@@ -8055,17 +8224,17 @@
         <v>161</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AC31" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="AD31" s="25" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="AE31" s="25"/>
       <c r="AK31" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8076,16 +8245,16 @@
         <v>260</v>
       </c>
       <c r="D32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H32" t="s">
         <v>206</v>
@@ -8094,34 +8263,37 @@
         <v>169</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="M32" t="s">
         <v>172</v>
       </c>
       <c r="N32" t="s">
+        <v>405</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="R32" t="s">
+        <v>408</v>
+      </c>
+      <c r="S32" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="T32" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="Q32" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="R32" t="s">
-        <v>412</v>
-      </c>
-      <c r="S32" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="T32" s="2" t="s">
-        <v>414</v>
+      <c r="V32" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="X32" s="28">
         <v>4397.05</v>
@@ -8132,28 +8304,28 @@
         <v>201</v>
       </c>
       <c r="AB32" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC32" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC32" s="31" t="s">
+      <c r="AD32" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="AD32" s="33" t="s">
-        <v>292</v>
-      </c>
       <c r="AE32" s="25" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AF32" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AG32" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="AH32" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AK32" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8164,16 +8336,16 @@
         <v>265</v>
       </c>
       <c r="D33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H33" t="s">
         <v>206</v>
@@ -8182,34 +8354,37 @@
         <v>169</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="M33" t="s">
         <v>172</v>
       </c>
       <c r="N33" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="R33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>459</v>
       </c>
       <c r="X33" s="28">
         <v>2195.5500000000002</v>
@@ -8220,22 +8395,22 @@
         <v>201</v>
       </c>
       <c r="AB33" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC33" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC33" s="31" t="s">
+      <c r="AD33" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="AD33" s="33" t="s">
-        <v>292</v>
-      </c>
       <c r="AE33" s="25" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="AF33" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="AK33" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8246,52 +8421,52 @@
         <v>266</v>
       </c>
       <c r="D34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I34" t="s">
         <v>169</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="M34" t="s">
         <v>172</v>
       </c>
       <c r="N34" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="R34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="X34" s="28">
         <v>1362.55</v>
@@ -8302,28 +8477,28 @@
         <v>201</v>
       </c>
       <c r="AB34" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC34" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AC34" s="31" t="s">
+      <c r="AD34" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="AD34" s="33" t="s">
-        <v>292</v>
-      </c>
       <c r="AE34" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF34" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="AG34" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AH34" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="AK34" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -8372,82 +8547,98 @@
     <hyperlink ref="K26" r:id="rId40" location="box_eventlist" xr:uid="{D9FB8F58-CCE6-4AB9-9554-7941A734BFB5}"/>
     <hyperlink ref="K25" r:id="rId41" xr:uid="{E5774072-115A-4C1D-AF74-2A6CA04CCBD8}"/>
     <hyperlink ref="AB25" r:id="rId42" xr:uid="{48422D63-E971-4F92-921A-A4DFE62BFD03}"/>
-    <hyperlink ref="AB26" r:id="rId43" xr:uid="{57F13425-9C42-4DA7-8F7C-11497F4C0A58}"/>
-    <hyperlink ref="AK15" r:id="rId44" xr:uid="{A10C35B7-E762-46BD-9CDD-B5AF14DEB810}"/>
-    <hyperlink ref="AK9" r:id="rId45" xr:uid="{F99707CB-8FE5-4C04-8E73-C23AECCB6875}"/>
-    <hyperlink ref="AK10:AK14" r:id="rId46" display="https://www.bfz.de/kontakt" xr:uid="{0B8F4342-1501-4BCB-B5E4-AF09F1763AE2}"/>
-    <hyperlink ref="AK16" r:id="rId47" xr:uid="{E76FB1AE-DC17-4E5E-A20A-B7BD7ECD9DC2}"/>
-    <hyperlink ref="AK17" r:id="rId48" xr:uid="{FB0D6304-97EB-46D5-A9F5-93B97833460F}"/>
-    <hyperlink ref="AK23" r:id="rId49" xr:uid="{2F7D02D7-B9E5-4B74-93A6-E758F6A9E280}"/>
-    <hyperlink ref="AK24" r:id="rId50" xr:uid="{674426C5-6AEC-4CF0-AF72-4CB19414FC5B}"/>
-    <hyperlink ref="AK25" r:id="rId51" xr:uid="{CAE8AEBB-01BB-48BE-9C19-376AA60572F3}"/>
-    <hyperlink ref="AK26" r:id="rId52" xr:uid="{8F39F751-2862-45C3-8CBC-EBCA38A00DCC}"/>
-    <hyperlink ref="AK27" r:id="rId53" xr:uid="{60CDBCF1-1E85-49D1-95A2-9D29F691911D}"/>
-    <hyperlink ref="K17" r:id="rId54" xr:uid="{D0DBF6BC-A6BF-4E02-AACC-1E80F71C2425}"/>
-    <hyperlink ref="L17" r:id="rId55" xr:uid="{91A3F409-610D-47AC-97BD-E798BA027F84}"/>
-    <hyperlink ref="K27" r:id="rId56" xr:uid="{24805552-1F93-48B4-9818-6ED1261BBD1E}"/>
-    <hyperlink ref="L27" r:id="rId57" xr:uid="{53C7F97E-A4A5-404B-9AA0-39D0B3F624D0}"/>
-    <hyperlink ref="AB27" r:id="rId58" xr:uid="{AD99EBB2-9A42-4CE8-B8F8-93C1DD00F620}"/>
-    <hyperlink ref="K3" r:id="rId59" xr:uid="{9327A321-37DB-4BF2-9F82-E7614A8CECC7}"/>
-    <hyperlink ref="K4" r:id="rId60" xr:uid="{9D1207A4-A274-4B77-AAA7-C0EA1AEF0808}"/>
-    <hyperlink ref="K5" r:id="rId61" xr:uid="{3D7E6130-BB3E-4FD5-9E89-7172F3ADD685}"/>
-    <hyperlink ref="K6" r:id="rId62" xr:uid="{C53C0317-C9D4-4DF6-ACFF-C811370ADF51}"/>
-    <hyperlink ref="K7" r:id="rId63" xr:uid="{9C12FCB6-CCB3-40AA-8424-9A76CAB8CBD0}"/>
-    <hyperlink ref="L3" r:id="rId64" xr:uid="{F4EE54C7-86F0-4194-9016-4958A638B80F}"/>
-    <hyperlink ref="L4" r:id="rId65" xr:uid="{2A066521-47A5-4E8D-98A7-BD9E2ACB72E1}"/>
-    <hyperlink ref="L5" r:id="rId66" xr:uid="{2D5273EE-BD97-4FBC-9731-2929C24E035D}"/>
-    <hyperlink ref="L6" r:id="rId67" xr:uid="{EDF8F773-F4D1-4960-B80C-D8A1B715ECEB}"/>
-    <hyperlink ref="L7" r:id="rId68" xr:uid="{96A71AAB-9E9A-4728-AB05-B44F70B2E88D}"/>
-    <hyperlink ref="K8" r:id="rId69" xr:uid="{24A5E069-5B4F-42E3-85C4-1AF80689987F}"/>
-    <hyperlink ref="L8" r:id="rId70" xr:uid="{2C7B6CAA-7398-4850-8D13-FB1E06CABD0B}"/>
-    <hyperlink ref="AK2" r:id="rId71" xr:uid="{4069FB99-6BFD-4632-A3A1-8C78A6464C04}"/>
-    <hyperlink ref="AK3:AK8" r:id="rId72" display="https://www.biwe-bbq.de/" xr:uid="{2B754280-4445-49A0-AE95-C546C1784657}"/>
-    <hyperlink ref="K18:K22" r:id="rId73" display="https://kurse.tuv.com/details/fachlagerist-m-w-d-teilqualifizierungen_ngtk8" xr:uid="{481B9E9A-5951-4929-9928-8BA443592823}"/>
-    <hyperlink ref="L18:L22" r:id="rId74" display="https://kurse.tuv.com/details/fachlagerist-m-w-d-teilqualifizierungen_ngtk8" xr:uid="{7BFCEEA7-EA9B-442B-BBCB-E05B950C3DD3}"/>
-    <hyperlink ref="L18" r:id="rId75" xr:uid="{34CB6AC6-589B-4659-B1EC-09C87B8E2DBF}"/>
-    <hyperlink ref="L19" r:id="rId76" xr:uid="{1BA0A695-FEB1-4ED3-9F5F-4132F488107C}"/>
-    <hyperlink ref="L20" r:id="rId77" xr:uid="{E22A6DEF-F969-457D-ABCE-BC049278C2E4}"/>
-    <hyperlink ref="L21" r:id="rId78" xr:uid="{AC50AEA0-1D1E-44C8-82B8-594DC6C72E9B}"/>
-    <hyperlink ref="L22" r:id="rId79" xr:uid="{B457A56F-20B9-4452-808A-FD4F996A609B}"/>
-    <hyperlink ref="AB17" r:id="rId80" xr:uid="{3E74DBD9-CB2B-432D-A7D3-C50081846512}"/>
-    <hyperlink ref="AB18" r:id="rId81" xr:uid="{0BE4408F-7964-483B-9C05-46F28E3AA94B}"/>
-    <hyperlink ref="AB19" r:id="rId82" xr:uid="{D660F09A-453A-4A3A-8CC3-D1BB1A21ACE2}"/>
-    <hyperlink ref="AB20" r:id="rId83" xr:uid="{E39B89A8-B5CF-4411-A0C7-BB3DABF0F429}"/>
-    <hyperlink ref="AB21" r:id="rId84" xr:uid="{E64568EA-B42A-4FC5-AAB0-338365E69C21}"/>
-    <hyperlink ref="AB22" r:id="rId85" xr:uid="{519D4AC8-BE94-410A-88B1-181406146EFF}"/>
-    <hyperlink ref="AK18:AK22" r:id="rId86" display="https://www.tuv.com/jobfit" xr:uid="{247D654F-AD98-42D7-B42A-F88D1BC59E2C}"/>
-    <hyperlink ref="L28" r:id="rId87" xr:uid="{C6058673-81DE-4A31-943B-468FD47A2447}"/>
-    <hyperlink ref="K28" r:id="rId88" xr:uid="{0852469A-DACA-47A7-812E-EC9CFDB01C2C}"/>
-    <hyperlink ref="AB28" r:id="rId89" xr:uid="{8DE27A13-08CB-4AC9-8355-D874776CE52D}"/>
-    <hyperlink ref="AK28" r:id="rId90" xr:uid="{3D7854CD-16E4-485A-8359-05D9BEF38F6A}"/>
-    <hyperlink ref="K32" r:id="rId91" xr:uid="{CF95DBBE-54DC-4037-9448-03DC05304A43}"/>
-    <hyperlink ref="L32" r:id="rId92" xr:uid="{89D8A758-9885-4755-B813-C8AF44DB4A85}"/>
-    <hyperlink ref="AB32" r:id="rId93" xr:uid="{F88AFA70-FEB4-40A0-A9D4-496D6BD735C1}"/>
-    <hyperlink ref="AK32" r:id="rId94" xr:uid="{E440215F-7763-46A9-AC2E-249AA8B22948}"/>
-    <hyperlink ref="K33" r:id="rId95" xr:uid="{F068538C-D850-4D79-A062-06910C13D8E0}"/>
-    <hyperlink ref="L33" r:id="rId96" xr:uid="{5473926C-3B4C-4300-8303-5C896CDE80F1}"/>
-    <hyperlink ref="AB33" r:id="rId97" xr:uid="{C93EB906-51C5-4D94-BF6E-2FD08576437F}"/>
-    <hyperlink ref="AK33" r:id="rId98" xr:uid="{5DACEF05-A133-487D-9495-88AE85CC9B40}"/>
-    <hyperlink ref="K34" r:id="rId99" xr:uid="{0622D9A8-2CF5-47B1-AE3F-A299E2475469}"/>
-    <hyperlink ref="L34" r:id="rId100" xr:uid="{12277F2F-6286-4E8F-AEEB-DB1049FFD1EF}"/>
-    <hyperlink ref="AB34" r:id="rId101" xr:uid="{C743E014-3894-4476-8216-163EAE873499}"/>
-    <hyperlink ref="AK34" r:id="rId102" xr:uid="{0517BAA0-8119-4BBC-935E-6358CB148F08}"/>
-    <hyperlink ref="L29" r:id="rId103" xr:uid="{B39A5727-4AA5-4AF9-975C-20A1836ECCA3}"/>
-    <hyperlink ref="K29" r:id="rId104" xr:uid="{7BFE051F-96F0-4BB4-A6D1-346C77FD2227}"/>
-    <hyperlink ref="K30" r:id="rId105" xr:uid="{C9D3256A-2D16-4469-88C8-F5FB2E8F12CA}"/>
-    <hyperlink ref="L30" r:id="rId106" xr:uid="{2A8830E0-69DF-476F-9461-1119DC926CA9}"/>
-    <hyperlink ref="L31" r:id="rId107" xr:uid="{3C2C025A-F330-4302-87A3-87350273D7C6}"/>
-    <hyperlink ref="K31" r:id="rId108" xr:uid="{DE9B6ADF-5598-4C2F-8895-090C0B719465}"/>
-    <hyperlink ref="AB31" r:id="rId109" xr:uid="{90FFA0E8-44AF-44AC-91DF-EC5EA2BD02D6}"/>
-    <hyperlink ref="AK31" r:id="rId110" xr:uid="{FBC98349-E58F-476F-9C64-AFF7A92A682F}"/>
-    <hyperlink ref="AK30" r:id="rId111" xr:uid="{8F951AC2-0E99-4071-965F-8368FD647468}"/>
-    <hyperlink ref="AK29" r:id="rId112" xr:uid="{A710276F-CD12-46ED-A703-49D7967E8767}"/>
+    <hyperlink ref="AK15" r:id="rId43" xr:uid="{A10C35B7-E762-46BD-9CDD-B5AF14DEB810}"/>
+    <hyperlink ref="AK9" r:id="rId44" xr:uid="{F99707CB-8FE5-4C04-8E73-C23AECCB6875}"/>
+    <hyperlink ref="AK10:AK14" r:id="rId45" display="https://www.bfz.de/kontakt" xr:uid="{0B8F4342-1501-4BCB-B5E4-AF09F1763AE2}"/>
+    <hyperlink ref="AK16" r:id="rId46" xr:uid="{E76FB1AE-DC17-4E5E-A20A-B7BD7ECD9DC2}"/>
+    <hyperlink ref="AK17" r:id="rId47" xr:uid="{FB0D6304-97EB-46D5-A9F5-93B97833460F}"/>
+    <hyperlink ref="AK23" r:id="rId48" xr:uid="{2F7D02D7-B9E5-4B74-93A6-E758F6A9E280}"/>
+    <hyperlink ref="AK24" r:id="rId49" xr:uid="{674426C5-6AEC-4CF0-AF72-4CB19414FC5B}"/>
+    <hyperlink ref="AK25" r:id="rId50" xr:uid="{CAE8AEBB-01BB-48BE-9C19-376AA60572F3}"/>
+    <hyperlink ref="AK26" r:id="rId51" xr:uid="{8F39F751-2862-45C3-8CBC-EBCA38A00DCC}"/>
+    <hyperlink ref="AK27" r:id="rId52" xr:uid="{60CDBCF1-1E85-49D1-95A2-9D29F691911D}"/>
+    <hyperlink ref="K17" r:id="rId53" xr:uid="{D0DBF6BC-A6BF-4E02-AACC-1E80F71C2425}"/>
+    <hyperlink ref="L17" r:id="rId54" xr:uid="{91A3F409-610D-47AC-97BD-E798BA027F84}"/>
+    <hyperlink ref="K27" r:id="rId55" xr:uid="{24805552-1F93-48B4-9818-6ED1261BBD1E}"/>
+    <hyperlink ref="L27" r:id="rId56" xr:uid="{53C7F97E-A4A5-404B-9AA0-39D0B3F624D0}"/>
+    <hyperlink ref="AB27" r:id="rId57" xr:uid="{AD99EBB2-9A42-4CE8-B8F8-93C1DD00F620}"/>
+    <hyperlink ref="K3" r:id="rId58" xr:uid="{9327A321-37DB-4BF2-9F82-E7614A8CECC7}"/>
+    <hyperlink ref="K4" r:id="rId59" xr:uid="{9D1207A4-A274-4B77-AAA7-C0EA1AEF0808}"/>
+    <hyperlink ref="K5" r:id="rId60" xr:uid="{3D7E6130-BB3E-4FD5-9E89-7172F3ADD685}"/>
+    <hyperlink ref="K6" r:id="rId61" xr:uid="{C53C0317-C9D4-4DF6-ACFF-C811370ADF51}"/>
+    <hyperlink ref="K7" r:id="rId62" xr:uid="{9C12FCB6-CCB3-40AA-8424-9A76CAB8CBD0}"/>
+    <hyperlink ref="L3" r:id="rId63" xr:uid="{F4EE54C7-86F0-4194-9016-4958A638B80F}"/>
+    <hyperlink ref="L4" r:id="rId64" xr:uid="{2A066521-47A5-4E8D-98A7-BD9E2ACB72E1}"/>
+    <hyperlink ref="L5" r:id="rId65" xr:uid="{2D5273EE-BD97-4FBC-9731-2929C24E035D}"/>
+    <hyperlink ref="L6" r:id="rId66" xr:uid="{EDF8F773-F4D1-4960-B80C-D8A1B715ECEB}"/>
+    <hyperlink ref="L7" r:id="rId67" xr:uid="{96A71AAB-9E9A-4728-AB05-B44F70B2E88D}"/>
+    <hyperlink ref="K8" r:id="rId68" xr:uid="{24A5E069-5B4F-42E3-85C4-1AF80689987F}"/>
+    <hyperlink ref="L8" r:id="rId69" xr:uid="{2C7B6CAA-7398-4850-8D13-FB1E06CABD0B}"/>
+    <hyperlink ref="AK2" r:id="rId70" xr:uid="{4069FB99-6BFD-4632-A3A1-8C78A6464C04}"/>
+    <hyperlink ref="AK3:AK8" r:id="rId71" display="https://www.biwe-bbq.de/" xr:uid="{2B754280-4445-49A0-AE95-C546C1784657}"/>
+    <hyperlink ref="K18:K22" r:id="rId72" display="https://kurse.tuv.com/details/fachlagerist-m-w-d-teilqualifizierungen_ngtk8" xr:uid="{481B9E9A-5951-4929-9928-8BA443592823}"/>
+    <hyperlink ref="L18:L22" r:id="rId73" display="https://kurse.tuv.com/details/fachlagerist-m-w-d-teilqualifizierungen_ngtk8" xr:uid="{7BFCEEA7-EA9B-442B-BBCB-E05B950C3DD3}"/>
+    <hyperlink ref="L18" r:id="rId74" xr:uid="{34CB6AC6-589B-4659-B1EC-09C87B8E2DBF}"/>
+    <hyperlink ref="L19" r:id="rId75" xr:uid="{1BA0A695-FEB1-4ED3-9F5F-4132F488107C}"/>
+    <hyperlink ref="L20" r:id="rId76" xr:uid="{E22A6DEF-F969-457D-ABCE-BC049278C2E4}"/>
+    <hyperlink ref="L21" r:id="rId77" xr:uid="{AC50AEA0-1D1E-44C8-82B8-594DC6C72E9B}"/>
+    <hyperlink ref="L22" r:id="rId78" xr:uid="{B457A56F-20B9-4452-808A-FD4F996A609B}"/>
+    <hyperlink ref="AB17" r:id="rId79" xr:uid="{3E74DBD9-CB2B-432D-A7D3-C50081846512}"/>
+    <hyperlink ref="AB18" r:id="rId80" xr:uid="{0BE4408F-7964-483B-9C05-46F28E3AA94B}"/>
+    <hyperlink ref="AB19" r:id="rId81" xr:uid="{D660F09A-453A-4A3A-8CC3-D1BB1A21ACE2}"/>
+    <hyperlink ref="AB20" r:id="rId82" xr:uid="{E39B89A8-B5CF-4411-A0C7-BB3DABF0F429}"/>
+    <hyperlink ref="AB21" r:id="rId83" xr:uid="{E64568EA-B42A-4FC5-AAB0-338365E69C21}"/>
+    <hyperlink ref="AB22" r:id="rId84" xr:uid="{519D4AC8-BE94-410A-88B1-181406146EFF}"/>
+    <hyperlink ref="AK18:AK22" r:id="rId85" display="https://www.tuv.com/jobfit" xr:uid="{247D654F-AD98-42D7-B42A-F88D1BC59E2C}"/>
+    <hyperlink ref="L28" r:id="rId86" xr:uid="{C6058673-81DE-4A31-943B-468FD47A2447}"/>
+    <hyperlink ref="K28" r:id="rId87" xr:uid="{0852469A-DACA-47A7-812E-EC9CFDB01C2C}"/>
+    <hyperlink ref="AB28" r:id="rId88" xr:uid="{8DE27A13-08CB-4AC9-8355-D874776CE52D}"/>
+    <hyperlink ref="AK28" r:id="rId89" xr:uid="{3D7854CD-16E4-485A-8359-05D9BEF38F6A}"/>
+    <hyperlink ref="K32" r:id="rId90" xr:uid="{CF95DBBE-54DC-4037-9448-03DC05304A43}"/>
+    <hyperlink ref="L32" r:id="rId91" xr:uid="{89D8A758-9885-4755-B813-C8AF44DB4A85}"/>
+    <hyperlink ref="AB32" r:id="rId92" xr:uid="{F88AFA70-FEB4-40A0-A9D4-496D6BD735C1}"/>
+    <hyperlink ref="AK32" r:id="rId93" xr:uid="{E440215F-7763-46A9-AC2E-249AA8B22948}"/>
+    <hyperlink ref="K33" r:id="rId94" xr:uid="{F068538C-D850-4D79-A062-06910C13D8E0}"/>
+    <hyperlink ref="L33" r:id="rId95" xr:uid="{5473926C-3B4C-4300-8303-5C896CDE80F1}"/>
+    <hyperlink ref="AB33" r:id="rId96" xr:uid="{C93EB906-51C5-4D94-BF6E-2FD08576437F}"/>
+    <hyperlink ref="AK33" r:id="rId97" xr:uid="{5DACEF05-A133-487D-9495-88AE85CC9B40}"/>
+    <hyperlink ref="K34" r:id="rId98" xr:uid="{0622D9A8-2CF5-47B1-AE3F-A299E2475469}"/>
+    <hyperlink ref="L34" r:id="rId99" xr:uid="{12277F2F-6286-4E8F-AEEB-DB1049FFD1EF}"/>
+    <hyperlink ref="AB34" r:id="rId100" xr:uid="{C743E014-3894-4476-8216-163EAE873499}"/>
+    <hyperlink ref="AK34" r:id="rId101" xr:uid="{0517BAA0-8119-4BBC-935E-6358CB148F08}"/>
+    <hyperlink ref="L29" r:id="rId102" xr:uid="{B39A5727-4AA5-4AF9-975C-20A1836ECCA3}"/>
+    <hyperlink ref="K29" r:id="rId103" xr:uid="{7BFE051F-96F0-4BB4-A6D1-346C77FD2227}"/>
+    <hyperlink ref="K30" r:id="rId104" xr:uid="{C9D3256A-2D16-4469-88C8-F5FB2E8F12CA}"/>
+    <hyperlink ref="L30" r:id="rId105" xr:uid="{2A8830E0-69DF-476F-9461-1119DC926CA9}"/>
+    <hyperlink ref="L31" r:id="rId106" xr:uid="{3C2C025A-F330-4302-87A3-87350273D7C6}"/>
+    <hyperlink ref="K31" r:id="rId107" xr:uid="{DE9B6ADF-5598-4C2F-8895-090C0B719465}"/>
+    <hyperlink ref="AB31" r:id="rId108" xr:uid="{90FFA0E8-44AF-44AC-91DF-EC5EA2BD02D6}"/>
+    <hyperlink ref="AK31" r:id="rId109" xr:uid="{FBC98349-E58F-476F-9C64-AFF7A92A682F}"/>
+    <hyperlink ref="AK30" r:id="rId110" xr:uid="{8F951AC2-0E99-4071-965F-8368FD647468}"/>
+    <hyperlink ref="AK29" r:id="rId111" xr:uid="{A710276F-CD12-46ED-A703-49D7967E8767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0a02612f-c061-4319-bfdb-b5863aa27d0a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100422B2238F8DAAD478C0837055D4C9439" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3cc5534cd780fd9e31c09b047b200ae0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8859808f-556d-416b-ba10-3a64d67cd7c4" xmlns:ns4="0a02612f-c061-4319-bfdb-b5863aa27d0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47912ec95e7c0f2f58d4b636259ebaea" ns3:_="" ns4:_="">
     <xsd:import namespace="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
@@ -8676,24 +8867,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9107FA45-FCDD-42C9-8B94-F455BA9BA50E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0a02612f-c061-4319-bfdb-b5863aa27d0a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0a02612f-c061-4319-bfdb-b5863aa27d0a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D77567D-EF8B-449E-AB9D-98DD6B7BC045}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7DC12C-AC0B-45A5-9CE7-33B2216F9746}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8710,29 +8909,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D77567D-EF8B-449E-AB9D-98DD6B7BC045}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9107FA45-FCDD-42C9-8B94-F455BA9BA50E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8859808f-556d-416b-ba10-3a64d67cd7c4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0a02612f-c061-4319-bfdb-b5863aa27d0a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>